<commit_message>
Update transmission to circuit miles and update costs
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -1,27 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF026065-DE5E-4768-BFAD-2F7855879C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="90" windowWidth="17220" windowHeight="8205"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="BTC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>BTC BAU Transmission Capacity</t>
   </si>
@@ -74,9 +108,6 @@
     <t>pixels</t>
   </si>
   <si>
-    <t>BAU Transmission Capacity (MW*miles)</t>
-  </si>
-  <si>
     <t>MW*miles</t>
   </si>
   <si>
@@ -90,12 +121,36 @@
   </si>
   <si>
     <t>and interpolate.</t>
+  </si>
+  <si>
+    <t>US Energy Information Administration</t>
+  </si>
+  <si>
+    <t>EIA study examines the role of high-voltage power lines in integrating renewables</t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/todayinenergy/detail.php?id=36393</t>
+  </si>
+  <si>
+    <t>BAU Transmission Capacity (circuit miles)</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Current Value</t>
+  </si>
+  <si>
+    <t>Indexed to 2018</t>
+  </si>
+  <si>
+    <t>2018 value from EIA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
@@ -124,12 +179,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -154,6 +215,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -176,20 +238,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>302260</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>102235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297382</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>137474</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>192607</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>67624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -208,8 +276,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4046220" y="1638300"/>
-          <a:ext cx="2331922" cy="3619814"/>
+          <a:off x="4798060" y="102235"/>
+          <a:ext cx="2328747" cy="3584889"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -297,6 +365,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -332,6 +417,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,49 +609,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="2">
         <v>2012</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{FF197175-E7A8-4C69-9B18-B36AE5DAEF78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -557,53 +694,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -612,10 +751,10 @@
         <v>150000000</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -624,10 +763,10 @@
         <v>200000000</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -636,15 +775,15 @@
         <v>175000000</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -655,7 +794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -666,16 +805,629 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="4">
         <f>B16/B15*50*10^6</f>
         <v>5319148.9361702129</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2010</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B12</f>
+        <v>175000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2050</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B12+B17</f>
+        <v>180319148.93617022</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2010</v>
+      </c>
+      <c r="B23">
+        <v>2011</v>
+      </c>
+      <c r="C23">
+        <v>2012</v>
+      </c>
+      <c r="D23">
+        <v>2013</v>
+      </c>
+      <c r="E23">
+        <v>2014</v>
+      </c>
+      <c r="F23">
+        <v>2015</v>
+      </c>
+      <c r="G23">
+        <v>2016</v>
+      </c>
+      <c r="H23">
+        <v>2017</v>
+      </c>
+      <c r="I23">
+        <v>2018</v>
+      </c>
+      <c r="J23">
+        <v>2019</v>
+      </c>
+      <c r="K23">
+        <v>2020</v>
+      </c>
+      <c r="L23">
+        <v>2021</v>
+      </c>
+      <c r="M23">
+        <v>2022</v>
+      </c>
+      <c r="N23">
+        <v>2023</v>
+      </c>
+      <c r="O23">
+        <v>2024</v>
+      </c>
+      <c r="P23">
+        <v>2025</v>
+      </c>
+      <c r="Q23">
+        <v>2026</v>
+      </c>
+      <c r="R23">
+        <v>2027</v>
+      </c>
+      <c r="S23">
+        <v>2028</v>
+      </c>
+      <c r="T23">
+        <v>2029</v>
+      </c>
+      <c r="U23">
+        <v>2030</v>
+      </c>
+      <c r="V23">
+        <v>2031</v>
+      </c>
+      <c r="W23">
+        <v>2032</v>
+      </c>
+      <c r="X23">
+        <v>2033</v>
+      </c>
+      <c r="Y23">
+        <v>2034</v>
+      </c>
+      <c r="Z23">
+        <v>2035</v>
+      </c>
+      <c r="AA23">
+        <v>2036</v>
+      </c>
+      <c r="AB23">
+        <v>2037</v>
+      </c>
+      <c r="AC23">
+        <v>2038</v>
+      </c>
+      <c r="AD23">
+        <v>2039</v>
+      </c>
+      <c r="AE23">
+        <v>2040</v>
+      </c>
+      <c r="AF23">
+        <v>2041</v>
+      </c>
+      <c r="AG23">
+        <v>2042</v>
+      </c>
+      <c r="AH23">
+        <v>2043</v>
+      </c>
+      <c r="AI23">
+        <v>2044</v>
+      </c>
+      <c r="AJ23">
+        <v>2045</v>
+      </c>
+      <c r="AK23">
+        <v>2046</v>
+      </c>
+      <c r="AL23">
+        <v>2047</v>
+      </c>
+      <c r="AM23">
+        <v>2048</v>
+      </c>
+      <c r="AN23">
+        <v>2049</v>
+      </c>
+      <c r="AO23">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" cm="1">
+        <f t="array" ref="A24">TREND($B$20:$B$21,$A$20:$A$21,A23)</f>
+        <v>175000000</v>
+      </c>
+      <c r="B24" s="4" cm="1">
+        <f t="array" ref="B24">TREND($B$20:$B$21,$A$20:$A$21,B23)</f>
+        <v>175132978.72340426</v>
+      </c>
+      <c r="C24" s="4" cm="1">
+        <f t="array" ref="C24">TREND($B$20:$B$21,$A$20:$A$21,C23)</f>
+        <v>175265957.44680852</v>
+      </c>
+      <c r="D24" s="4" cm="1">
+        <f t="array" ref="D24">TREND($B$20:$B$21,$A$20:$A$21,D23)</f>
+        <v>175398936.17021278</v>
+      </c>
+      <c r="E24" s="4" cm="1">
+        <f t="array" ref="E24">TREND($B$20:$B$21,$A$20:$A$21,E23)</f>
+        <v>175531914.893617</v>
+      </c>
+      <c r="F24" s="4" cm="1">
+        <f t="array" ref="F24">TREND($B$20:$B$21,$A$20:$A$21,F23)</f>
+        <v>175664893.61702126</v>
+      </c>
+      <c r="G24" s="4" cm="1">
+        <f t="array" ref="G24">TREND($B$20:$B$21,$A$20:$A$21,G23)</f>
+        <v>175797872.34042552</v>
+      </c>
+      <c r="H24" s="4" cm="1">
+        <f t="array" ref="H24">TREND($B$20:$B$21,$A$20:$A$21,H23)</f>
+        <v>175930851.06382978</v>
+      </c>
+      <c r="I24" s="4" cm="1">
+        <f t="array" ref="I24">TREND($B$20:$B$21,$A$20:$A$21,I23)</f>
+        <v>176063829.78723404</v>
+      </c>
+      <c r="J24" s="4" cm="1">
+        <f t="array" ref="J24">TREND($B$20:$B$21,$A$20:$A$21,J23)</f>
+        <v>176196808.5106383</v>
+      </c>
+      <c r="K24" s="4" cm="1">
+        <f t="array" ref="K24">TREND($B$20:$B$21,$A$20:$A$21,K23)</f>
+        <v>176329787.23404253</v>
+      </c>
+      <c r="L24" s="4" cm="1">
+        <f t="array" ref="L24">TREND($B$20:$B$21,$A$20:$A$21,L23)</f>
+        <v>176462765.95744681</v>
+      </c>
+      <c r="M24" s="4" cm="1">
+        <f t="array" ref="M24">TREND($B$20:$B$21,$A$20:$A$21,M23)</f>
+        <v>176595744.68085104</v>
+      </c>
+      <c r="N24" s="4" cm="1">
+        <f t="array" ref="N24">TREND($B$20:$B$21,$A$20:$A$21,N23)</f>
+        <v>176728723.40425533</v>
+      </c>
+      <c r="O24" s="4" cm="1">
+        <f t="array" ref="O24">TREND($B$20:$B$21,$A$20:$A$21,O23)</f>
+        <v>176861702.12765956</v>
+      </c>
+      <c r="P24" s="4" cm="1">
+        <f t="array" ref="P24">TREND($B$20:$B$21,$A$20:$A$21,P23)</f>
+        <v>176994680.85106385</v>
+      </c>
+      <c r="Q24" s="4" cm="1">
+        <f t="array" ref="Q24">TREND($B$20:$B$21,$A$20:$A$21,Q23)</f>
+        <v>177127659.57446808</v>
+      </c>
+      <c r="R24" s="4" cm="1">
+        <f t="array" ref="R24">TREND($B$20:$B$21,$A$20:$A$21,R23)</f>
+        <v>177260638.29787236</v>
+      </c>
+      <c r="S24" s="4" cm="1">
+        <f t="array" ref="S24">TREND($B$20:$B$21,$A$20:$A$21,S23)</f>
+        <v>177393617.02127659</v>
+      </c>
+      <c r="T24" s="4" cm="1">
+        <f t="array" ref="T24">TREND($B$20:$B$21,$A$20:$A$21,T23)</f>
+        <v>177526595.74468082</v>
+      </c>
+      <c r="U24" s="4" cm="1">
+        <f t="array" ref="U24">TREND($B$20:$B$21,$A$20:$A$21,U23)</f>
+        <v>177659574.46808511</v>
+      </c>
+      <c r="V24" s="4" cm="1">
+        <f t="array" ref="V24">TREND($B$20:$B$21,$A$20:$A$21,V23)</f>
+        <v>177792553.19148934</v>
+      </c>
+      <c r="W24" s="4" cm="1">
+        <f t="array" ref="W24">TREND($B$20:$B$21,$A$20:$A$21,W23)</f>
+        <v>177925531.91489363</v>
+      </c>
+      <c r="X24" s="4" cm="1">
+        <f t="array" ref="X24">TREND($B$20:$B$21,$A$20:$A$21,X23)</f>
+        <v>178058510.63829786</v>
+      </c>
+      <c r="Y24" s="4" cm="1">
+        <f t="array" ref="Y24">TREND($B$20:$B$21,$A$20:$A$21,Y23)</f>
+        <v>178191489.36170214</v>
+      </c>
+      <c r="Z24" s="4" cm="1">
+        <f t="array" ref="Z24">TREND($B$20:$B$21,$A$20:$A$21,Z23)</f>
+        <v>178324468.08510637</v>
+      </c>
+      <c r="AA24" s="4" cm="1">
+        <f t="array" ref="AA24">TREND($B$20:$B$21,$A$20:$A$21,AA23)</f>
+        <v>178457446.80851066</v>
+      </c>
+      <c r="AB24" s="4" cm="1">
+        <f t="array" ref="AB24">TREND($B$20:$B$21,$A$20:$A$21,AB23)</f>
+        <v>178590425.53191489</v>
+      </c>
+      <c r="AC24" s="4" cm="1">
+        <f t="array" ref="AC24">TREND($B$20:$B$21,$A$20:$A$21,AC23)</f>
+        <v>178723404.25531918</v>
+      </c>
+      <c r="AD24" s="4" cm="1">
+        <f t="array" ref="AD24">TREND($B$20:$B$21,$A$20:$A$21,AD23)</f>
+        <v>178856382.97872341</v>
+      </c>
+      <c r="AE24" s="4" cm="1">
+        <f t="array" ref="AE24">TREND($B$20:$B$21,$A$20:$A$21,AE23)</f>
+        <v>178989361.70212764</v>
+      </c>
+      <c r="AF24" s="4" cm="1">
+        <f t="array" ref="AF24">TREND($B$20:$B$21,$A$20:$A$21,AF23)</f>
+        <v>179122340.42553192</v>
+      </c>
+      <c r="AG24" s="4" cm="1">
+        <f t="array" ref="AG24">TREND($B$20:$B$21,$A$20:$A$21,AG23)</f>
+        <v>179255319.14893615</v>
+      </c>
+      <c r="AH24" s="4" cm="1">
+        <f t="array" ref="AH24">TREND($B$20:$B$21,$A$20:$A$21,AH23)</f>
+        <v>179388297.87234044</v>
+      </c>
+      <c r="AI24" s="4" cm="1">
+        <f t="array" ref="AI24">TREND($B$20:$B$21,$A$20:$A$21,AI23)</f>
+        <v>179521276.59574467</v>
+      </c>
+      <c r="AJ24" s="4" cm="1">
+        <f t="array" ref="AJ24">TREND($B$20:$B$21,$A$20:$A$21,AJ23)</f>
+        <v>179654255.31914896</v>
+      </c>
+      <c r="AK24" s="4" cm="1">
+        <f t="array" ref="AK24">TREND($B$20:$B$21,$A$20:$A$21,AK23)</f>
+        <v>179787234.04255319</v>
+      </c>
+      <c r="AL24" s="4" cm="1">
+        <f t="array" ref="AL24">TREND($B$20:$B$21,$A$20:$A$21,AL23)</f>
+        <v>179920212.76595747</v>
+      </c>
+      <c r="AM24" s="4" cm="1">
+        <f t="array" ref="AM24">TREND($B$20:$B$21,$A$20:$A$21,AM23)</f>
+        <v>180053191.4893617</v>
+      </c>
+      <c r="AN24" s="4" cm="1">
+        <f t="array" ref="AN24">TREND($B$20:$B$21,$A$20:$A$21,AN23)</f>
+        <v>180186170.21276593</v>
+      </c>
+      <c r="AO24" s="4" cm="1">
+        <f t="array" ref="AO24">TREND($B$20:$B$21,$A$20:$A$21,AO23)</f>
+        <v>180319148.93617022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2010</v>
+      </c>
+      <c r="B27">
+        <v>2011</v>
+      </c>
+      <c r="C27">
+        <v>2012</v>
+      </c>
+      <c r="D27">
+        <v>2013</v>
+      </c>
+      <c r="E27">
+        <v>2014</v>
+      </c>
+      <c r="F27">
+        <v>2015</v>
+      </c>
+      <c r="G27">
+        <v>2016</v>
+      </c>
+      <c r="H27">
+        <v>2017</v>
+      </c>
+      <c r="I27">
+        <v>2018</v>
+      </c>
+      <c r="J27">
+        <v>2019</v>
+      </c>
+      <c r="K27">
+        <v>2020</v>
+      </c>
+      <c r="L27">
+        <v>2021</v>
+      </c>
+      <c r="M27">
+        <v>2022</v>
+      </c>
+      <c r="N27">
+        <v>2023</v>
+      </c>
+      <c r="O27">
+        <v>2024</v>
+      </c>
+      <c r="P27">
+        <v>2025</v>
+      </c>
+      <c r="Q27">
+        <v>2026</v>
+      </c>
+      <c r="R27">
+        <v>2027</v>
+      </c>
+      <c r="S27">
+        <v>2028</v>
+      </c>
+      <c r="T27">
+        <v>2029</v>
+      </c>
+      <c r="U27">
+        <v>2030</v>
+      </c>
+      <c r="V27">
+        <v>2031</v>
+      </c>
+      <c r="W27">
+        <v>2032</v>
+      </c>
+      <c r="X27">
+        <v>2033</v>
+      </c>
+      <c r="Y27">
+        <v>2034</v>
+      </c>
+      <c r="Z27">
+        <v>2035</v>
+      </c>
+      <c r="AA27">
+        <v>2036</v>
+      </c>
+      <c r="AB27">
+        <v>2037</v>
+      </c>
+      <c r="AC27">
+        <v>2038</v>
+      </c>
+      <c r="AD27">
+        <v>2039</v>
+      </c>
+      <c r="AE27">
+        <v>2040</v>
+      </c>
+      <c r="AF27">
+        <v>2041</v>
+      </c>
+      <c r="AG27">
+        <v>2042</v>
+      </c>
+      <c r="AH27">
+        <v>2043</v>
+      </c>
+      <c r="AI27">
+        <v>2044</v>
+      </c>
+      <c r="AJ27">
+        <v>2045</v>
+      </c>
+      <c r="AK27">
+        <v>2046</v>
+      </c>
+      <c r="AL27">
+        <v>2047</v>
+      </c>
+      <c r="AM27">
+        <v>2048</v>
+      </c>
+      <c r="AN27">
+        <v>2049</v>
+      </c>
+      <c r="AO27">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <f>A24/$I$24</f>
+        <v>0.9939577039274925</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" ref="B28:AO28" si="0">B24/$I$24</f>
+        <v>0.99471299093655596</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99546827794561943</v>
+      </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99622356495468289</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99697885196374614</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9977341389728096</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99848942598187307</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99924471299093653</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0007552870090635</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0015105740181267</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0022658610271904</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0030211480362536</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0037764350453173</v>
+      </c>
+      <c r="O28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0045317220543806</v>
+      </c>
+      <c r="P28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0052870090634443</v>
+      </c>
+      <c r="Q28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0060422960725075</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0067975830815712</v>
+      </c>
+      <c r="S28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0075528700906344</v>
+      </c>
+      <c r="T28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0083081570996977</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0090634441087614</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0098187311178246</v>
+      </c>
+      <c r="W28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0105740181268883</v>
+      </c>
+      <c r="X28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0113293051359515</v>
+      </c>
+      <c r="Y28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0120845921450152</v>
+      </c>
+      <c r="Z28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0128398791540785</v>
+      </c>
+      <c r="AA28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0135951661631422</v>
+      </c>
+      <c r="AB28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0143504531722054</v>
+      </c>
+      <c r="AC28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0151057401812691</v>
+      </c>
+      <c r="AD28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0158610271903323</v>
+      </c>
+      <c r="AE28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0166163141993956</v>
+      </c>
+      <c r="AF28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0173716012084593</v>
+      </c>
+      <c r="AG28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0181268882175225</v>
+      </c>
+      <c r="AH28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0188821752265862</v>
+      </c>
+      <c r="AI28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0196374622356494</v>
+      </c>
+      <c r="AJ28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0203927492447131</v>
+      </c>
+      <c r="AK28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0211480362537764</v>
+      </c>
+      <c r="AL28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0219033232628401</v>
+      </c>
+      <c r="AM28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0226586102719033</v>
+      </c>
+      <c r="AN28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0234138972809665</v>
+      </c>
+      <c r="AO28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0241691842900302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>700000</v>
       </c>
     </row>
   </sheetData>
@@ -685,314 +1437,258 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="42" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="34" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="B1">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="C1">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="D1">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="E1">
-        <v>2013</v>
+        <v>2021</v>
       </c>
       <c r="F1">
-        <v>2014</v>
+        <v>2022</v>
       </c>
       <c r="G1">
-        <v>2015</v>
+        <v>2023</v>
       </c>
       <c r="H1">
-        <v>2016</v>
+        <v>2024</v>
       </c>
       <c r="I1">
-        <v>2017</v>
+        <v>2025</v>
       </c>
       <c r="J1">
-        <v>2018</v>
+        <v>2026</v>
       </c>
       <c r="K1">
-        <v>2019</v>
+        <v>2027</v>
       </c>
       <c r="L1">
-        <v>2020</v>
+        <v>2028</v>
       </c>
       <c r="M1">
-        <v>2021</v>
+        <v>2029</v>
       </c>
       <c r="N1">
-        <v>2022</v>
+        <v>2030</v>
       </c>
       <c r="O1">
-        <v>2023</v>
+        <v>2031</v>
       </c>
       <c r="P1">
-        <v>2024</v>
+        <v>2032</v>
       </c>
       <c r="Q1">
-        <v>2025</v>
+        <v>2033</v>
       </c>
       <c r="R1">
-        <v>2026</v>
+        <v>2034</v>
       </c>
       <c r="S1">
-        <v>2027</v>
+        <v>2035</v>
       </c>
       <c r="T1">
-        <v>2028</v>
+        <v>2036</v>
       </c>
       <c r="U1">
-        <v>2029</v>
+        <v>2037</v>
       </c>
       <c r="V1">
-        <v>2030</v>
+        <v>2038</v>
       </c>
       <c r="W1">
-        <v>2031</v>
+        <v>2039</v>
       </c>
       <c r="X1">
-        <v>2032</v>
+        <v>2040</v>
       </c>
       <c r="Y1">
-        <v>2033</v>
+        <v>2041</v>
       </c>
       <c r="Z1">
-        <v>2034</v>
+        <v>2042</v>
       </c>
       <c r="AA1">
-        <v>2035</v>
+        <v>2043</v>
       </c>
       <c r="AB1">
-        <v>2036</v>
+        <v>2044</v>
       </c>
       <c r="AC1">
-        <v>2037</v>
+        <v>2045</v>
       </c>
       <c r="AD1">
-        <v>2038</v>
+        <v>2046</v>
       </c>
       <c r="AE1">
-        <v>2039</v>
+        <v>2047</v>
       </c>
       <c r="AF1">
-        <v>2040</v>
+        <v>2048</v>
       </c>
       <c r="AG1">
-        <v>2041</v>
+        <v>2049</v>
       </c>
       <c r="AH1">
-        <v>2042</v>
-      </c>
-      <c r="AI1">
-        <v>2043</v>
-      </c>
-      <c r="AJ1">
-        <v>2044</v>
-      </c>
-      <c r="AK1">
-        <v>2045</v>
-      </c>
-      <c r="AL1">
-        <v>2046</v>
-      </c>
-      <c r="AM1">
-        <v>2047</v>
-      </c>
-      <c r="AN1">
-        <v>2048</v>
-      </c>
-      <c r="AO1">
-        <v>2049</v>
-      </c>
-      <c r="AP1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5">
-        <f>Data!B12</f>
-        <v>175000000</v>
+        <f>Data!I28*Data!$B$30</f>
+        <v>700000</v>
       </c>
       <c r="C2" s="5">
-        <f>B2+Data!$B$17/(2050-2010)</f>
-        <v>175132978.72340426</v>
+        <f>Data!J28*Data!$B$30</f>
+        <v>700528.70090634446</v>
       </c>
       <c r="D2" s="5">
-        <f>C2+Data!$B$17/(2050-2010)</f>
-        <v>175265957.44680852</v>
+        <f>Data!K28*Data!$B$30</f>
+        <v>701057.40181268868</v>
       </c>
       <c r="E2" s="5">
-        <f>D2+Data!$B$17/(2050-2010)</f>
-        <v>175398936.17021278</v>
+        <f>Data!L28*Data!$B$30</f>
+        <v>701586.10271903325</v>
       </c>
       <c r="F2" s="5">
-        <f>E2+Data!$B$17/(2050-2010)</f>
-        <v>175531914.89361703</v>
+        <f>Data!M28*Data!$B$30</f>
+        <v>702114.80362537759</v>
       </c>
       <c r="G2" s="5">
-        <f>F2+Data!$B$17/(2050-2010)</f>
-        <v>175664893.61702129</v>
+        <f>Data!N28*Data!$B$30</f>
+        <v>702643.50453172217</v>
       </c>
       <c r="H2" s="5">
-        <f>G2+Data!$B$17/(2050-2010)</f>
-        <v>175797872.34042555</v>
+        <f>Data!O28*Data!$B$30</f>
+        <v>703172.20543806639</v>
       </c>
       <c r="I2" s="5">
-        <f>H2+Data!$B$17/(2050-2010)</f>
-        <v>175930851.06382981</v>
+        <f>Data!P28*Data!$B$30</f>
+        <v>703700.90634441096</v>
       </c>
       <c r="J2" s="5">
-        <f>I2+Data!$B$17/(2050-2010)</f>
-        <v>176063829.78723407</v>
+        <f>Data!Q28*Data!$B$30</f>
+        <v>704229.6072507553</v>
       </c>
       <c r="K2" s="5">
-        <f>J2+Data!$B$17/(2050-2010)</f>
-        <v>176196808.51063833</v>
+        <f>Data!R28*Data!$B$30</f>
+        <v>704758.30815709988</v>
       </c>
       <c r="L2" s="5">
-        <f>K2+Data!$B$17/(2050-2010)</f>
-        <v>176329787.23404258</v>
+        <f>Data!S28*Data!$B$30</f>
+        <v>705287.0090634441</v>
       </c>
       <c r="M2" s="5">
-        <f>L2+Data!$B$17/(2050-2010)</f>
-        <v>176462765.95744684</v>
+        <f>Data!T28*Data!$B$30</f>
+        <v>705815.70996978832</v>
       </c>
       <c r="N2" s="5">
-        <f>M2+Data!$B$17/(2050-2010)</f>
-        <v>176595744.6808511</v>
+        <f>Data!U28*Data!$B$30</f>
+        <v>706344.41087613301</v>
       </c>
       <c r="O2" s="5">
-        <f>N2+Data!$B$17/(2050-2010)</f>
-        <v>176728723.40425536</v>
+        <f>Data!V28*Data!$B$30</f>
+        <v>706873.11178247724</v>
       </c>
       <c r="P2" s="5">
-        <f>O2+Data!$B$17/(2050-2010)</f>
-        <v>176861702.12765962</v>
+        <f>Data!W28*Data!$B$30</f>
+        <v>707401.81268882181</v>
       </c>
       <c r="Q2" s="5">
-        <f>P2+Data!$B$17/(2050-2010)</f>
-        <v>176994680.85106388</v>
+        <f>Data!X28*Data!$B$30</f>
+        <v>707930.51359516603</v>
       </c>
       <c r="R2" s="5">
-        <f>Q2+Data!$B$17/(2050-2010)</f>
-        <v>177127659.57446814</v>
+        <f>Data!Y28*Data!$B$30</f>
+        <v>708459.21450151061</v>
       </c>
       <c r="S2" s="5">
-        <f>R2+Data!$B$17/(2050-2010)</f>
-        <v>177260638.29787239</v>
+        <f>Data!Z28*Data!$B$30</f>
+        <v>708987.91540785495</v>
       </c>
       <c r="T2" s="5">
-        <f>S2+Data!$B$17/(2050-2010)</f>
-        <v>177393617.02127665</v>
+        <f>Data!AA28*Data!$B$30</f>
+        <v>709516.61631419952</v>
       </c>
       <c r="U2" s="5">
-        <f>T2+Data!$B$17/(2050-2010)</f>
-        <v>177526595.74468091</v>
+        <f>Data!AB28*Data!$B$30</f>
+        <v>710045.31722054374</v>
       </c>
       <c r="V2" s="5">
-        <f>U2+Data!$B$17/(2050-2010)</f>
-        <v>177659574.46808517</v>
+        <f>Data!AC28*Data!$B$30</f>
+        <v>710574.01812688832</v>
       </c>
       <c r="W2" s="5">
-        <f>V2+Data!$B$17/(2050-2010)</f>
-        <v>177792553.19148943</v>
+        <f>Data!AD28*Data!$B$30</f>
+        <v>711102.71903323266</v>
       </c>
       <c r="X2" s="5">
-        <f>W2+Data!$B$17/(2050-2010)</f>
-        <v>177925531.91489369</v>
+        <f>Data!AE28*Data!$B$30</f>
+        <v>711631.41993957688</v>
       </c>
       <c r="Y2" s="5">
-        <f>X2+Data!$B$17/(2050-2010)</f>
-        <v>178058510.63829795</v>
+        <f>Data!AF28*Data!$B$30</f>
+        <v>712160.12084592145</v>
       </c>
       <c r="Z2" s="5">
-        <f>Y2+Data!$B$17/(2050-2010)</f>
-        <v>178191489.3617022</v>
+        <f>Data!AG28*Data!$B$30</f>
+        <v>712688.82175226579</v>
       </c>
       <c r="AA2" s="5">
-        <f>Z2+Data!$B$17/(2050-2010)</f>
-        <v>178324468.08510646</v>
+        <f>Data!AH28*Data!$B$30</f>
+        <v>713217.52265861037</v>
       </c>
       <c r="AB2" s="5">
-        <f>AA2+Data!$B$17/(2050-2010)</f>
-        <v>178457446.80851072</v>
+        <f>Data!AI28*Data!$B$30</f>
+        <v>713746.22356495459</v>
       </c>
       <c r="AC2" s="5">
-        <f>AB2+Data!$B$17/(2050-2010)</f>
-        <v>178590425.53191498</v>
+        <f>Data!AJ28*Data!$B$30</f>
+        <v>714274.92447129916</v>
       </c>
       <c r="AD2" s="5">
-        <f>AC2+Data!$B$17/(2050-2010)</f>
-        <v>178723404.25531924</v>
+        <f>Data!AK28*Data!$B$30</f>
+        <v>714803.6253776435</v>
       </c>
       <c r="AE2" s="5">
-        <f>AD2+Data!$B$17/(2050-2010)</f>
-        <v>178856382.9787235</v>
+        <f>Data!AL28*Data!$B$30</f>
+        <v>715332.32628398808</v>
       </c>
       <c r="AF2" s="5">
-        <f>AE2+Data!$B$17/(2050-2010)</f>
-        <v>178989361.70212775</v>
+        <f>Data!AM28*Data!$B$30</f>
+        <v>715861.0271903323</v>
       </c>
       <c r="AG2" s="5">
-        <f>AF2+Data!$B$17/(2050-2010)</f>
-        <v>179122340.42553201</v>
+        <f>Data!AN28*Data!$B$30</f>
+        <v>716389.72809667652</v>
       </c>
       <c r="AH2" s="5">
-        <f>AG2+Data!$B$17/(2050-2010)</f>
-        <v>179255319.14893627</v>
-      </c>
-      <c r="AI2" s="5">
-        <f>AH2+Data!$B$17/(2050-2010)</f>
-        <v>179388297.87234053</v>
-      </c>
-      <c r="AJ2" s="5">
-        <f>AI2+Data!$B$17/(2050-2010)</f>
-        <v>179521276.59574479</v>
-      </c>
-      <c r="AK2" s="5">
-        <f>AJ2+Data!$B$17/(2050-2010)</f>
-        <v>179654255.31914905</v>
-      </c>
-      <c r="AL2" s="5">
-        <f>AK2+Data!$B$17/(2050-2010)</f>
-        <v>179787234.04255331</v>
-      </c>
-      <c r="AM2" s="5">
-        <f>AL2+Data!$B$17/(2050-2010)</f>
-        <v>179920212.76595756</v>
-      </c>
-      <c r="AN2" s="5">
-        <f>AM2+Data!$B$17/(2050-2010)</f>
-        <v>180053191.48936182</v>
-      </c>
-      <c r="AO2" s="5">
-        <f>AN2+Data!$B$17/(2050-2010)</f>
-        <v>180186170.21276608</v>
-      </c>
-      <c r="AP2" s="5">
-        <f>AO2+Data!$B$17/(2050-2010)</f>
-        <v>180319148.93617034</v>
+        <f>Data!AO28*Data!$B$30</f>
+        <v>716918.42900302121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add increased transmission from IIJA funding to BAU
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF026065-DE5E-4768-BFAD-2F7855879C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F8E2A8-C454-4BE7-8E86-9179A9BB67F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="BTC" sheetId="3" r:id="rId3"/>
+    <sheet name="IIJA" sheetId="4" r:id="rId3"/>
+    <sheet name="BTC" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>BTC BAU Transmission Capacity</t>
   </si>
@@ -144,7 +145,46 @@
     <t>Indexed to 2018</t>
   </si>
   <si>
-    <t>2018 value from EIA</t>
+    <t>Infrastructure Investment and Jobs Act Effects</t>
+  </si>
+  <si>
+    <t>Transmission Projects Ready to Go: Plugging Into America's Untapped Renewable Resources</t>
+  </si>
+  <si>
+    <t>Americans for a Clean Energy Grid and Grid Strategies</t>
+  </si>
+  <si>
+    <t>Page 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cleanenergygrid.org/wp-content/uploads/2019/04/Transmission-Projects-Ready-to-Go-Final.pdf </t>
+  </si>
+  <si>
+    <t>Number of MW-miles proposed</t>
+  </si>
+  <si>
+    <t>Proposed investment</t>
+  </si>
+  <si>
+    <t>IIJA Funding</t>
+  </si>
+  <si>
+    <t>Number of MW-miles installed through 2030*</t>
+  </si>
+  <si>
+    <t>*assume funding is available through 2026, but due to the long nature of transmission projects,</t>
+  </si>
+  <si>
+    <t>some lines may come online after 2026</t>
+  </si>
+  <si>
+    <t>2018 value from EIA (citcuit-miles)</t>
+  </si>
+  <si>
+    <t>additional capacity (MW-miles)</t>
+  </si>
+  <si>
+    <t>additional capacity (circuit-miles)</t>
   </si>
 </sst>
 </file>
@@ -154,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +214,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,24 +249,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -610,143 +668,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B5" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B11" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{FF197175-E7A8-4C69-9B18-B36AE5DAEF78}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{070385A7-390D-4C16-A425-72A247234116}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AO30"/>
+  <dimension ref="A1:AO33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.453125" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="2">
         <f>150*10^6</f>
         <v>150000000</v>
       </c>
@@ -754,11 +849,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <f>200*10^6</f>
         <v>200000000</v>
       </c>
@@ -766,11 +861,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <f>AVERAGE(B10:B11)</f>
         <v>175000000</v>
       </c>
@@ -778,12 +873,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -794,7 +889,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -805,11 +900,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <f>B16/B15*50*10^6</f>
         <v>5319148.9361702129</v>
       </c>
@@ -817,25 +912,25 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2010</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="2">
         <f>B12</f>
         <v>175000000</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2050</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="2">
         <f>B12+B17</f>
         <v>180319148.93617022</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -960,178 +1055,178 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" cm="1">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" cm="1">
         <f t="array" ref="A24">TREND($B$20:$B$21,$A$20:$A$21,A23)</f>
         <v>175000000</v>
       </c>
-      <c r="B24" s="4" cm="1">
+      <c r="B24" s="2" cm="1">
         <f t="array" ref="B24">TREND($B$20:$B$21,$A$20:$A$21,B23)</f>
         <v>175132978.72340426</v>
       </c>
-      <c r="C24" s="4" cm="1">
+      <c r="C24" s="2" cm="1">
         <f t="array" ref="C24">TREND($B$20:$B$21,$A$20:$A$21,C23)</f>
         <v>175265957.44680852</v>
       </c>
-      <c r="D24" s="4" cm="1">
+      <c r="D24" s="2" cm="1">
         <f t="array" ref="D24">TREND($B$20:$B$21,$A$20:$A$21,D23)</f>
         <v>175398936.17021278</v>
       </c>
-      <c r="E24" s="4" cm="1">
+      <c r="E24" s="2" cm="1">
         <f t="array" ref="E24">TREND($B$20:$B$21,$A$20:$A$21,E23)</f>
         <v>175531914.893617</v>
       </c>
-      <c r="F24" s="4" cm="1">
+      <c r="F24" s="2" cm="1">
         <f t="array" ref="F24">TREND($B$20:$B$21,$A$20:$A$21,F23)</f>
         <v>175664893.61702126</v>
       </c>
-      <c r="G24" s="4" cm="1">
+      <c r="G24" s="2" cm="1">
         <f t="array" ref="G24">TREND($B$20:$B$21,$A$20:$A$21,G23)</f>
         <v>175797872.34042552</v>
       </c>
-      <c r="H24" s="4" cm="1">
+      <c r="H24" s="2" cm="1">
         <f t="array" ref="H24">TREND($B$20:$B$21,$A$20:$A$21,H23)</f>
         <v>175930851.06382978</v>
       </c>
-      <c r="I24" s="4" cm="1">
+      <c r="I24" s="2" cm="1">
         <f t="array" ref="I24">TREND($B$20:$B$21,$A$20:$A$21,I23)</f>
         <v>176063829.78723404</v>
       </c>
-      <c r="J24" s="4" cm="1">
+      <c r="J24" s="2" cm="1">
         <f t="array" ref="J24">TREND($B$20:$B$21,$A$20:$A$21,J23)</f>
         <v>176196808.5106383</v>
       </c>
-      <c r="K24" s="4" cm="1">
+      <c r="K24" s="2" cm="1">
         <f t="array" ref="K24">TREND($B$20:$B$21,$A$20:$A$21,K23)</f>
         <v>176329787.23404253</v>
       </c>
-      <c r="L24" s="4" cm="1">
+      <c r="L24" s="2" cm="1">
         <f t="array" ref="L24">TREND($B$20:$B$21,$A$20:$A$21,L23)</f>
         <v>176462765.95744681</v>
       </c>
-      <c r="M24" s="4" cm="1">
+      <c r="M24" s="2" cm="1">
         <f t="array" ref="M24">TREND($B$20:$B$21,$A$20:$A$21,M23)</f>
         <v>176595744.68085104</v>
       </c>
-      <c r="N24" s="4" cm="1">
+      <c r="N24" s="2" cm="1">
         <f t="array" ref="N24">TREND($B$20:$B$21,$A$20:$A$21,N23)</f>
         <v>176728723.40425533</v>
       </c>
-      <c r="O24" s="4" cm="1">
+      <c r="O24" s="2" cm="1">
         <f t="array" ref="O24">TREND($B$20:$B$21,$A$20:$A$21,O23)</f>
         <v>176861702.12765956</v>
       </c>
-      <c r="P24" s="4" cm="1">
+      <c r="P24" s="2" cm="1">
         <f t="array" ref="P24">TREND($B$20:$B$21,$A$20:$A$21,P23)</f>
         <v>176994680.85106385</v>
       </c>
-      <c r="Q24" s="4" cm="1">
+      <c r="Q24" s="2" cm="1">
         <f t="array" ref="Q24">TREND($B$20:$B$21,$A$20:$A$21,Q23)</f>
         <v>177127659.57446808</v>
       </c>
-      <c r="R24" s="4" cm="1">
+      <c r="R24" s="2" cm="1">
         <f t="array" ref="R24">TREND($B$20:$B$21,$A$20:$A$21,R23)</f>
         <v>177260638.29787236</v>
       </c>
-      <c r="S24" s="4" cm="1">
+      <c r="S24" s="2" cm="1">
         <f t="array" ref="S24">TREND($B$20:$B$21,$A$20:$A$21,S23)</f>
         <v>177393617.02127659</v>
       </c>
-      <c r="T24" s="4" cm="1">
+      <c r="T24" s="2" cm="1">
         <f t="array" ref="T24">TREND($B$20:$B$21,$A$20:$A$21,T23)</f>
         <v>177526595.74468082</v>
       </c>
-      <c r="U24" s="4" cm="1">
+      <c r="U24" s="2" cm="1">
         <f t="array" ref="U24">TREND($B$20:$B$21,$A$20:$A$21,U23)</f>
         <v>177659574.46808511</v>
       </c>
-      <c r="V24" s="4" cm="1">
+      <c r="V24" s="2" cm="1">
         <f t="array" ref="V24">TREND($B$20:$B$21,$A$20:$A$21,V23)</f>
         <v>177792553.19148934</v>
       </c>
-      <c r="W24" s="4" cm="1">
+      <c r="W24" s="2" cm="1">
         <f t="array" ref="W24">TREND($B$20:$B$21,$A$20:$A$21,W23)</f>
         <v>177925531.91489363</v>
       </c>
-      <c r="X24" s="4" cm="1">
+      <c r="X24" s="2" cm="1">
         <f t="array" ref="X24">TREND($B$20:$B$21,$A$20:$A$21,X23)</f>
         <v>178058510.63829786</v>
       </c>
-      <c r="Y24" s="4" cm="1">
+      <c r="Y24" s="2" cm="1">
         <f t="array" ref="Y24">TREND($B$20:$B$21,$A$20:$A$21,Y23)</f>
         <v>178191489.36170214</v>
       </c>
-      <c r="Z24" s="4" cm="1">
+      <c r="Z24" s="2" cm="1">
         <f t="array" ref="Z24">TREND($B$20:$B$21,$A$20:$A$21,Z23)</f>
         <v>178324468.08510637</v>
       </c>
-      <c r="AA24" s="4" cm="1">
+      <c r="AA24" s="2" cm="1">
         <f t="array" ref="AA24">TREND($B$20:$B$21,$A$20:$A$21,AA23)</f>
         <v>178457446.80851066</v>
       </c>
-      <c r="AB24" s="4" cm="1">
+      <c r="AB24" s="2" cm="1">
         <f t="array" ref="AB24">TREND($B$20:$B$21,$A$20:$A$21,AB23)</f>
         <v>178590425.53191489</v>
       </c>
-      <c r="AC24" s="4" cm="1">
+      <c r="AC24" s="2" cm="1">
         <f t="array" ref="AC24">TREND($B$20:$B$21,$A$20:$A$21,AC23)</f>
         <v>178723404.25531918</v>
       </c>
-      <c r="AD24" s="4" cm="1">
+      <c r="AD24" s="2" cm="1">
         <f t="array" ref="AD24">TREND($B$20:$B$21,$A$20:$A$21,AD23)</f>
         <v>178856382.97872341</v>
       </c>
-      <c r="AE24" s="4" cm="1">
+      <c r="AE24" s="2" cm="1">
         <f t="array" ref="AE24">TREND($B$20:$B$21,$A$20:$A$21,AE23)</f>
         <v>178989361.70212764</v>
       </c>
-      <c r="AF24" s="4" cm="1">
+      <c r="AF24" s="2" cm="1">
         <f t="array" ref="AF24">TREND($B$20:$B$21,$A$20:$A$21,AF23)</f>
         <v>179122340.42553192</v>
       </c>
-      <c r="AG24" s="4" cm="1">
+      <c r="AG24" s="2" cm="1">
         <f t="array" ref="AG24">TREND($B$20:$B$21,$A$20:$A$21,AG23)</f>
         <v>179255319.14893615</v>
       </c>
-      <c r="AH24" s="4" cm="1">
+      <c r="AH24" s="2" cm="1">
         <f t="array" ref="AH24">TREND($B$20:$B$21,$A$20:$A$21,AH23)</f>
         <v>179388297.87234044</v>
       </c>
-      <c r="AI24" s="4" cm="1">
+      <c r="AI24" s="2" cm="1">
         <f t="array" ref="AI24">TREND($B$20:$B$21,$A$20:$A$21,AI23)</f>
         <v>179521276.59574467</v>
       </c>
-      <c r="AJ24" s="4" cm="1">
+      <c r="AJ24" s="2" cm="1">
         <f t="array" ref="AJ24">TREND($B$20:$B$21,$A$20:$A$21,AJ23)</f>
         <v>179654255.31914896</v>
       </c>
-      <c r="AK24" s="4" cm="1">
+      <c r="AK24" s="2" cm="1">
         <f t="array" ref="AK24">TREND($B$20:$B$21,$A$20:$A$21,AK23)</f>
         <v>179787234.04255319</v>
       </c>
-      <c r="AL24" s="4" cm="1">
+      <c r="AL24" s="2" cm="1">
         <f t="array" ref="AL24">TREND($B$20:$B$21,$A$20:$A$21,AL23)</f>
         <v>179920212.76595747</v>
       </c>
-      <c r="AM24" s="4" cm="1">
+      <c r="AM24" s="2" cm="1">
         <f t="array" ref="AM24">TREND($B$20:$B$21,$A$20:$A$21,AM23)</f>
         <v>180053191.4893617</v>
       </c>
-      <c r="AN24" s="4" cm="1">
+      <c r="AN24" s="2" cm="1">
         <f t="array" ref="AN24">TREND($B$20:$B$21,$A$20:$A$21,AN23)</f>
         <v>180186170.21276593</v>
       </c>
-      <c r="AO24" s="4" cm="1">
+      <c r="AO24" s="2" cm="1">
         <f t="array" ref="AO24">TREND($B$20:$B$21,$A$20:$A$21,AO23)</f>
         <v>180319148.93617022</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2010</v>
       </c>
@@ -1256,179 +1351,185 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
-      <c r="A28" s="4">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <f>A24/$I$24</f>
         <v>0.9939577039274925</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="2">
         <f t="shared" ref="B28:AO28" si="0">B24/$I$24</f>
         <v>0.99471299093655596</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>0.99546827794561943</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>0.99622356495468289</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <f t="shared" si="0"/>
         <v>0.99697885196374614</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="2">
         <f t="shared" si="0"/>
         <v>0.9977341389728096</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="2">
         <f t="shared" si="0"/>
         <v>0.99848942598187307</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="2">
         <f t="shared" si="0"/>
         <v>0.99924471299093653</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="2">
         <f t="shared" si="0"/>
         <v>1.0007552870090635</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="2">
         <f t="shared" si="0"/>
         <v>1.0015105740181267</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="2">
         <f t="shared" si="0"/>
         <v>1.0022658610271904</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28" s="2">
         <f t="shared" si="0"/>
         <v>1.0030211480362536</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28" s="2">
         <f t="shared" si="0"/>
         <v>1.0037764350453173</v>
       </c>
-      <c r="O28" s="4">
+      <c r="O28" s="2">
         <f t="shared" si="0"/>
         <v>1.0045317220543806</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P28" s="2">
         <f t="shared" si="0"/>
         <v>1.0052870090634443</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="Q28" s="2">
         <f t="shared" si="0"/>
         <v>1.0060422960725075</v>
       </c>
-      <c r="R28" s="4">
+      <c r="R28" s="2">
         <f t="shared" si="0"/>
         <v>1.0067975830815712</v>
       </c>
-      <c r="S28" s="4">
+      <c r="S28" s="2">
         <f t="shared" si="0"/>
         <v>1.0075528700906344</v>
       </c>
-      <c r="T28" s="4">
+      <c r="T28" s="2">
         <f t="shared" si="0"/>
         <v>1.0083081570996977</v>
       </c>
-      <c r="U28" s="4">
+      <c r="U28" s="2">
         <f t="shared" si="0"/>
         <v>1.0090634441087614</v>
       </c>
-      <c r="V28" s="4">
+      <c r="V28" s="2">
         <f t="shared" si="0"/>
         <v>1.0098187311178246</v>
       </c>
-      <c r="W28" s="4">
+      <c r="W28" s="2">
         <f t="shared" si="0"/>
         <v>1.0105740181268883</v>
       </c>
-      <c r="X28" s="4">
+      <c r="X28" s="2">
         <f t="shared" si="0"/>
         <v>1.0113293051359515</v>
       </c>
-      <c r="Y28" s="4">
+      <c r="Y28" s="2">
         <f t="shared" si="0"/>
         <v>1.0120845921450152</v>
       </c>
-      <c r="Z28" s="4">
+      <c r="Z28" s="2">
         <f t="shared" si="0"/>
         <v>1.0128398791540785</v>
       </c>
-      <c r="AA28" s="4">
+      <c r="AA28" s="2">
         <f t="shared" si="0"/>
         <v>1.0135951661631422</v>
       </c>
-      <c r="AB28" s="4">
+      <c r="AB28" s="2">
         <f t="shared" si="0"/>
         <v>1.0143504531722054</v>
       </c>
-      <c r="AC28" s="4">
+      <c r="AC28" s="2">
         <f t="shared" si="0"/>
         <v>1.0151057401812691</v>
       </c>
-      <c r="AD28" s="4">
+      <c r="AD28" s="2">
         <f t="shared" si="0"/>
         <v>1.0158610271903323</v>
       </c>
-      <c r="AE28" s="4">
+      <c r="AE28" s="2">
         <f t="shared" si="0"/>
         <v>1.0166163141993956</v>
       </c>
-      <c r="AF28" s="4">
+      <c r="AF28" s="2">
         <f t="shared" si="0"/>
         <v>1.0173716012084593</v>
       </c>
-      <c r="AG28" s="4">
+      <c r="AG28" s="2">
         <f t="shared" si="0"/>
         <v>1.0181268882175225</v>
       </c>
-      <c r="AH28" s="4">
+      <c r="AH28" s="2">
         <f t="shared" si="0"/>
         <v>1.0188821752265862</v>
       </c>
-      <c r="AI28" s="4">
+      <c r="AI28" s="2">
         <f t="shared" si="0"/>
         <v>1.0196374622356494</v>
       </c>
-      <c r="AJ28" s="4">
+      <c r="AJ28" s="2">
         <f t="shared" si="0"/>
         <v>1.0203927492447131</v>
       </c>
-      <c r="AK28" s="4">
+      <c r="AK28" s="2">
         <f t="shared" si="0"/>
         <v>1.0211480362537764</v>
       </c>
-      <c r="AL28" s="4">
+      <c r="AL28" s="2">
         <f t="shared" si="0"/>
         <v>1.0219033232628401</v>
       </c>
-      <c r="AM28" s="4">
+      <c r="AM28" s="2">
         <f t="shared" si="0"/>
         <v>1.0226586102719033</v>
       </c>
-      <c r="AN28" s="4">
+      <c r="AN28" s="2">
         <f t="shared" si="0"/>
         <v>1.0234138972809665</v>
       </c>
-      <c r="AO28" s="4">
+      <c r="AO28" s="2">
         <f t="shared" si="0"/>
         <v>1.0241691842900302</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>700000</v>
       </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U31" s="2"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,23 +1538,426 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A8E9EE-75BB-4C67-BE26-F56AE2DF869D}">
+  <dimension ref="A1:AD14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1">
+        <f>17*10^6</f>
+        <v>17000000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <f>33*10^9</f>
+        <v>33000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <f>500000000*5</f>
+        <v>2500000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2">
+        <f>B1/B2*B3</f>
+        <v>1287878.7878787878</v>
+      </c>
+      <c r="D4" s="9">
+        <f>B4/Data!U24</f>
+        <v>7.2491380874614405E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>2023</v>
+      </c>
+      <c r="D9">
+        <v>2024</v>
+      </c>
+      <c r="E9">
+        <v>2025</v>
+      </c>
+      <c r="F9">
+        <v>2026</v>
+      </c>
+      <c r="G9">
+        <v>2027</v>
+      </c>
+      <c r="H9">
+        <v>2028</v>
+      </c>
+      <c r="I9">
+        <v>2029</v>
+      </c>
+      <c r="J9">
+        <v>2030</v>
+      </c>
+      <c r="K9">
+        <v>2031</v>
+      </c>
+      <c r="L9">
+        <v>2032</v>
+      </c>
+      <c r="M9">
+        <v>2033</v>
+      </c>
+      <c r="N9">
+        <v>2034</v>
+      </c>
+      <c r="O9">
+        <v>2035</v>
+      </c>
+      <c r="P9">
+        <v>2036</v>
+      </c>
+      <c r="Q9">
+        <v>2037</v>
+      </c>
+      <c r="R9">
+        <v>2038</v>
+      </c>
+      <c r="S9">
+        <v>2039</v>
+      </c>
+      <c r="T9">
+        <v>2040</v>
+      </c>
+      <c r="U9">
+        <v>2041</v>
+      </c>
+      <c r="V9">
+        <v>2042</v>
+      </c>
+      <c r="W9">
+        <v>2043</v>
+      </c>
+      <c r="X9">
+        <v>2044</v>
+      </c>
+      <c r="Y9">
+        <v>2045</v>
+      </c>
+      <c r="Z9">
+        <v>2046</v>
+      </c>
+      <c r="AA9">
+        <v>2047</v>
+      </c>
+      <c r="AB9">
+        <v>2048</v>
+      </c>
+      <c r="AC9">
+        <v>2049</v>
+      </c>
+      <c r="AD9">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="2">
+        <f>$B$4/9</f>
+        <v>143097.6430976431</v>
+      </c>
+      <c r="C10" s="2">
+        <f>$B$4/9+B10</f>
+        <v>286195.2861952862</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" ref="D10:J10" si="0">$B$4/9+C10</f>
+        <v>429292.9292929293</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>572390.5723905724</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>715488.21548821544</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>858585.85858585848</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
+        <v>1001683.5016835015</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="0"/>
+        <v>1144781.1447811446</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="0"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="K10" s="2">
+        <f>$J$10</f>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10:AD10" si="1">$J$10</f>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="U10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="W10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="Y10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="Z10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="AA10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="AB10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="AC10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="AD10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2">
+        <f>B10/Data!$B$24*Data!$B$30</f>
+        <v>571.95595540318402</v>
+      </c>
+      <c r="C11" s="2">
+        <f>C10/Data!$B$24*Data!$B$30</f>
+        <v>1143.911910806368</v>
+      </c>
+      <c r="D11" s="2">
+        <f>D10/Data!$B$24*Data!$B$30</f>
+        <v>1715.8678662095519</v>
+      </c>
+      <c r="E11" s="2">
+        <f>E10/Data!$B$24*Data!$B$30</f>
+        <v>2287.8238216127361</v>
+      </c>
+      <c r="F11" s="2">
+        <f>F10/Data!$B$24*Data!$B$30</f>
+        <v>2859.7797770159195</v>
+      </c>
+      <c r="G11" s="2">
+        <f>G10/Data!$B$24*Data!$B$30</f>
+        <v>3431.7357324191034</v>
+      </c>
+      <c r="H11" s="2">
+        <f>H10/Data!$B$24*Data!$B$30</f>
+        <v>4003.6916878222869</v>
+      </c>
+      <c r="I11" s="2">
+        <f>I10/Data!$B$24*Data!$B$30</f>
+        <v>4575.6476432254703</v>
+      </c>
+      <c r="J11" s="2">
+        <f>J10/Data!$B$24*Data!$B$30</f>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="K11" s="2">
+        <f>$J$11</f>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" ref="L11:AD11" si="2">$J$11</f>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="U11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="W11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="Y11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="Z11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="AA11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="AB11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="AC11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="2"/>
+        <v>5147.6035986286543</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K14" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="34" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="34" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2018</v>
       </c>
@@ -1554,142 +2058,145 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <f>Data!I28*Data!$B$30</f>
         <v>700000</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <f>Data!J28*Data!$B$30</f>
         <v>700528.70090634446</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <f>Data!K28*Data!$B$30</f>
         <v>701057.40181268868</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="3">
         <f>Data!L28*Data!$B$30</f>
         <v>701586.10271903325</v>
       </c>
-      <c r="F2" s="5">
-        <f>Data!M28*Data!$B$30</f>
-        <v>702114.80362537759</v>
-      </c>
-      <c r="G2" s="5">
-        <f>Data!N28*Data!$B$30</f>
-        <v>702643.50453172217</v>
-      </c>
-      <c r="H2" s="5">
-        <f>Data!O28*Data!$B$30</f>
-        <v>703172.20543806639</v>
-      </c>
-      <c r="I2" s="5">
-        <f>Data!P28*Data!$B$30</f>
-        <v>703700.90634441096</v>
-      </c>
-      <c r="J2" s="5">
-        <f>Data!Q28*Data!$B$30</f>
-        <v>704229.6072507553</v>
-      </c>
-      <c r="K2" s="5">
-        <f>Data!R28*Data!$B$30</f>
-        <v>704758.30815709988</v>
-      </c>
-      <c r="L2" s="5">
-        <f>Data!S28*Data!$B$30</f>
-        <v>705287.0090634441</v>
-      </c>
-      <c r="M2" s="5">
-        <f>Data!T28*Data!$B$30</f>
-        <v>705815.70996978832</v>
-      </c>
-      <c r="N2" s="5">
-        <f>Data!U28*Data!$B$30</f>
-        <v>706344.41087613301</v>
-      </c>
-      <c r="O2" s="5">
-        <f>Data!V28*Data!$B$30</f>
-        <v>706873.11178247724</v>
-      </c>
-      <c r="P2" s="5">
-        <f>Data!W28*Data!$B$30</f>
-        <v>707401.81268882181</v>
-      </c>
-      <c r="Q2" s="5">
-        <f>Data!X28*Data!$B$30</f>
-        <v>707930.51359516603</v>
-      </c>
-      <c r="R2" s="5">
-        <f>Data!Y28*Data!$B$30</f>
-        <v>708459.21450151061</v>
-      </c>
-      <c r="S2" s="5">
-        <f>Data!Z28*Data!$B$30</f>
-        <v>708987.91540785495</v>
-      </c>
-      <c r="T2" s="5">
-        <f>Data!AA28*Data!$B$30</f>
-        <v>709516.61631419952</v>
-      </c>
-      <c r="U2" s="5">
-        <f>Data!AB28*Data!$B$30</f>
-        <v>710045.31722054374</v>
-      </c>
-      <c r="V2" s="5">
-        <f>Data!AC28*Data!$B$30</f>
-        <v>710574.01812688832</v>
-      </c>
-      <c r="W2" s="5">
-        <f>Data!AD28*Data!$B$30</f>
-        <v>711102.71903323266</v>
-      </c>
-      <c r="X2" s="5">
-        <f>Data!AE28*Data!$B$30</f>
-        <v>711631.41993957688</v>
-      </c>
-      <c r="Y2" s="5">
-        <f>Data!AF28*Data!$B$30</f>
-        <v>712160.12084592145</v>
-      </c>
-      <c r="Z2" s="5">
-        <f>Data!AG28*Data!$B$30</f>
-        <v>712688.82175226579</v>
-      </c>
-      <c r="AA2" s="5">
-        <f>Data!AH28*Data!$B$30</f>
-        <v>713217.52265861037</v>
-      </c>
-      <c r="AB2" s="5">
-        <f>Data!AI28*Data!$B$30</f>
-        <v>713746.22356495459</v>
-      </c>
-      <c r="AC2" s="5">
-        <f>Data!AJ28*Data!$B$30</f>
-        <v>714274.92447129916</v>
-      </c>
-      <c r="AD2" s="5">
-        <f>Data!AK28*Data!$B$30</f>
-        <v>714803.6253776435</v>
-      </c>
-      <c r="AE2" s="5">
-        <f>Data!AL28*Data!$B$30</f>
-        <v>715332.32628398808</v>
-      </c>
-      <c r="AF2" s="5">
-        <f>Data!AM28*Data!$B$30</f>
-        <v>715861.0271903323</v>
-      </c>
-      <c r="AG2" s="5">
-        <f>Data!AN28*Data!$B$30</f>
-        <v>716389.72809667652</v>
-      </c>
-      <c r="AH2" s="5">
-        <f>Data!AO28*Data!$B$30</f>
-        <v>716918.42900302121</v>
-      </c>
+      <c r="F2" s="3">
+        <f>Data!M28*Data!$B$30+IIJA!B11</f>
+        <v>702686.75958078075</v>
+      </c>
+      <c r="G2" s="3">
+        <f>Data!N28*Data!$B$30+IIJA!C11</f>
+        <v>703787.41644252848</v>
+      </c>
+      <c r="H2" s="3">
+        <f>Data!O28*Data!$B$30+IIJA!D11</f>
+        <v>704888.07330427598</v>
+      </c>
+      <c r="I2" s="3">
+        <f>Data!P28*Data!$B$30+IIJA!E11</f>
+        <v>705988.73016602371</v>
+      </c>
+      <c r="J2" s="3">
+        <f>Data!Q28*Data!$B$30+IIJA!F11</f>
+        <v>707089.38702777121</v>
+      </c>
+      <c r="K2" s="3">
+        <f>Data!R28*Data!$B$30+IIJA!G11</f>
+        <v>708190.04388951894</v>
+      </c>
+      <c r="L2" s="3">
+        <f>Data!S28*Data!$B$30+IIJA!H11</f>
+        <v>709290.70075126644</v>
+      </c>
+      <c r="M2" s="3">
+        <f>Data!T28*Data!$B$30+IIJA!I11</f>
+        <v>710391.35761301382</v>
+      </c>
+      <c r="N2" s="3">
+        <f>Data!U28*Data!$B$30+IIJA!J11</f>
+        <v>711492.01447476167</v>
+      </c>
+      <c r="O2" s="3">
+        <f>Data!V28*Data!$B$30+IIJA!K11</f>
+        <v>712020.7153811059</v>
+      </c>
+      <c r="P2" s="3">
+        <f>Data!W28*Data!$B$30+IIJA!L11</f>
+        <v>712549.41628745047</v>
+      </c>
+      <c r="Q2" s="3">
+        <f>Data!X28*Data!$B$30+IIJA!M11</f>
+        <v>713078.11719379469</v>
+      </c>
+      <c r="R2" s="3">
+        <f>Data!Y28*Data!$B$30+IIJA!N11</f>
+        <v>713606.81810013927</v>
+      </c>
+      <c r="S2" s="3">
+        <f>Data!Z28*Data!$B$30+IIJA!O11</f>
+        <v>714135.51900648361</v>
+      </c>
+      <c r="T2" s="3">
+        <f>Data!AA28*Data!$B$30+IIJA!P11</f>
+        <v>714664.21991282818</v>
+      </c>
+      <c r="U2" s="3">
+        <f>Data!AB28*Data!$B$30+IIJA!Q11</f>
+        <v>715192.9208191724</v>
+      </c>
+      <c r="V2" s="3">
+        <f>Data!AC28*Data!$B$30+IIJA!R11</f>
+        <v>715721.62172551698</v>
+      </c>
+      <c r="W2" s="3">
+        <f>Data!AD28*Data!$B$30+IIJA!S11</f>
+        <v>716250.32263186132</v>
+      </c>
+      <c r="X2" s="3">
+        <f>Data!AE28*Data!$B$30+IIJA!T11</f>
+        <v>716779.02353820554</v>
+      </c>
+      <c r="Y2" s="3">
+        <f>Data!AF28*Data!$B$30+IIJA!U11</f>
+        <v>717307.72444455011</v>
+      </c>
+      <c r="Z2" s="3">
+        <f>Data!AG28*Data!$B$30+IIJA!V11</f>
+        <v>717836.42535089445</v>
+      </c>
+      <c r="AA2" s="3">
+        <f>Data!AH28*Data!$B$30+IIJA!W11</f>
+        <v>718365.12625723903</v>
+      </c>
+      <c r="AB2" s="3">
+        <f>Data!AI28*Data!$B$30+IIJA!X11</f>
+        <v>718893.82716358325</v>
+      </c>
+      <c r="AC2" s="3">
+        <f>Data!AJ28*Data!$B$30+IIJA!Y11</f>
+        <v>719422.52806992782</v>
+      </c>
+      <c r="AD2" s="3">
+        <f>Data!AK28*Data!$B$30+IIJA!Z11</f>
+        <v>719951.22897627216</v>
+      </c>
+      <c r="AE2" s="3">
+        <f>Data!AL28*Data!$B$30+IIJA!AA11</f>
+        <v>720479.92988261674</v>
+      </c>
+      <c r="AF2" s="3">
+        <f>Data!AM28*Data!$B$30+IIJA!AB11</f>
+        <v>721008.63078896096</v>
+      </c>
+      <c r="AG2" s="3">
+        <f>Data!AN28*Data!$B$30+IIJA!AC11</f>
+        <v>721537.33169530518</v>
+      </c>
+      <c r="AH2" s="3">
+        <f>Data!AO28*Data!$B$30+IIJA!AD11</f>
+        <v>722066.03260164987</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="N4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Use new data source for transmission
</commit_message>
<xml_diff>
--- a/InputData/elec/BTC/BAU Transmission Capacity.xlsx
+++ b/InputData/elec/BTC/BAU Transmission Capacity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\BTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\elec\BTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F8E2A8-C454-4BE7-8E86-9179A9BB67F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7EED0E4-3621-4CED-AA03-E0C0C4F7BD07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>BTC BAU Transmission Capacity</t>
   </si>
@@ -124,30 +124,9 @@
     <t>and interpolate.</t>
   </si>
   <si>
-    <t>US Energy Information Administration</t>
-  </si>
-  <si>
-    <t>EIA study examines the role of high-voltage power lines in integrating renewables</t>
-  </si>
-  <si>
-    <t>https://www.eia.gov/todayinenergy/detail.php?id=36393</t>
-  </si>
-  <si>
-    <t>BAU Transmission Capacity (circuit miles)</t>
-  </si>
-  <si>
     <t>Scaling</t>
   </si>
   <si>
-    <t>Current Value</t>
-  </si>
-  <si>
-    <t>Indexed to 2018</t>
-  </si>
-  <si>
-    <t>Infrastructure Investment and Jobs Act Effects</t>
-  </si>
-  <si>
     <t>Transmission Projects Ready to Go: Plugging Into America's Untapped Renewable Resources</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t>Page 4</t>
   </si>
   <si>
-    <t xml:space="preserve">https://cleanenergygrid.org/wp-content/uploads/2019/04/Transmission-Projects-Ready-to-Go-Final.pdf </t>
-  </si>
-  <si>
     <t>Number of MW-miles proposed</t>
   </si>
   <si>
@@ -178,13 +154,25 @@
     <t>some lines may come online after 2026</t>
   </si>
   <si>
-    <t>2018 value from EIA (citcuit-miles)</t>
-  </si>
-  <si>
     <t>additional capacity (MW-miles)</t>
   </si>
   <si>
-    <t>additional capacity (circuit-miles)</t>
+    <t>Transmission Growth</t>
+  </si>
+  <si>
+    <t>Indexed to 2020</t>
+  </si>
+  <si>
+    <t>2021 Transmission Value</t>
+  </si>
+  <si>
+    <t>https://cleanenergygrid.org/wp-content/uploads/2019/04/Transmission-Projects-Ready-to-Go-Final.pdf</t>
+  </si>
+  <si>
+    <t>Current Value and Infrastructure Investment and Jobs Act Effects</t>
+  </si>
+  <si>
+    <t>BAU Transmission Capacity (MW-miles)</t>
   </si>
 </sst>
 </file>
@@ -298,13 +286,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>302260</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>102235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>192607</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>67624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -668,868 +656,778 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="6">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="6">
         <v>2012</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
-        <v>2021</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>32</v>
-      </c>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{FF197175-E7A8-4C69-9B18-B36AE5DAEF78}"/>
-    <hyperlink ref="B20" r:id="rId2" xr:uid="{070385A7-390D-4C16-A425-72A247234116}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{FF197175-E7A8-4C69-9B18-B36AE5DAEF78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AO33"/>
+  <dimension ref="A1:AO36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B11" s="2">
         <f>150*10^6</f>
         <v>150000000</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B12" s="2">
         <f>200*10^6</f>
         <v>200000000</v>
       </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
-        <f>AVERAGE(B10:B11)</f>
-        <v>175000000</v>
-      </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <f>AVERAGE(B11:B12)</f>
+        <v>175000000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>141</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2">
-        <f>B16/B15*50*10^6</f>
+      <c r="B18" s="2">
+        <f>B17/B16*50*10^6</f>
         <v>5319148.9361702129</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>2010</v>
       </c>
-      <c r="B20" s="2">
-        <f>B12</f>
+      <c r="B21" s="2">
+        <f>B13</f>
         <v>175000000</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>2050</v>
       </c>
-      <c r="B21" s="2">
-        <f>B12+B17</f>
+      <c r="B22" s="2">
+        <f>B13+B18</f>
         <v>180319148.93617022</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>2010</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>2011</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>2012</v>
       </c>
-      <c r="D23">
+      <c r="D24">
         <v>2013</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>2014</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>2015</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>2016</v>
       </c>
-      <c r="H23">
+      <c r="H24">
         <v>2017</v>
       </c>
-      <c r="I23">
+      <c r="I24">
         <v>2018</v>
       </c>
-      <c r="J23">
+      <c r="J24">
         <v>2019</v>
       </c>
-      <c r="K23">
+      <c r="K24">
         <v>2020</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <v>2021</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>2022</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>2023</v>
       </c>
-      <c r="O23">
+      <c r="O24">
         <v>2024</v>
       </c>
-      <c r="P23">
+      <c r="P24">
         <v>2025</v>
       </c>
-      <c r="Q23">
+      <c r="Q24">
         <v>2026</v>
       </c>
-      <c r="R23">
+      <c r="R24">
         <v>2027</v>
       </c>
-      <c r="S23">
+      <c r="S24">
         <v>2028</v>
       </c>
-      <c r="T23">
+      <c r="T24">
         <v>2029</v>
       </c>
-      <c r="U23">
+      <c r="U24">
         <v>2030</v>
       </c>
-      <c r="V23">
+      <c r="V24">
         <v>2031</v>
       </c>
-      <c r="W23">
+      <c r="W24">
         <v>2032</v>
       </c>
-      <c r="X23">
+      <c r="X24">
         <v>2033</v>
       </c>
-      <c r="Y23">
+      <c r="Y24">
         <v>2034</v>
       </c>
-      <c r="Z23">
+      <c r="Z24">
         <v>2035</v>
       </c>
-      <c r="AA23">
+      <c r="AA24">
         <v>2036</v>
       </c>
-      <c r="AB23">
+      <c r="AB24">
         <v>2037</v>
       </c>
-      <c r="AC23">
+      <c r="AC24">
         <v>2038</v>
       </c>
-      <c r="AD23">
+      <c r="AD24">
         <v>2039</v>
       </c>
-      <c r="AE23">
+      <c r="AE24">
         <v>2040</v>
       </c>
-      <c r="AF23">
+      <c r="AF24">
         <v>2041</v>
       </c>
-      <c r="AG23">
+      <c r="AG24">
         <v>2042</v>
       </c>
-      <c r="AH23">
+      <c r="AH24">
         <v>2043</v>
       </c>
-      <c r="AI23">
+      <c r="AI24">
         <v>2044</v>
       </c>
-      <c r="AJ23">
+      <c r="AJ24">
         <v>2045</v>
       </c>
-      <c r="AK23">
+      <c r="AK24">
         <v>2046</v>
       </c>
-      <c r="AL23">
+      <c r="AL24">
         <v>2047</v>
       </c>
-      <c r="AM23">
+      <c r="AM24">
         <v>2048</v>
       </c>
-      <c r="AN23">
+      <c r="AN24">
         <v>2049</v>
       </c>
-      <c r="AO23">
+      <c r="AO24">
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" cm="1">
-        <f t="array" ref="A24">TREND($B$20:$B$21,$A$20:$A$21,A23)</f>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" cm="1">
+        <f t="array" ref="A25">TREND($B$21:$B$22,$A$21:$A$22,A24)</f>
         <v>175000000</v>
       </c>
-      <c r="B24" s="2" cm="1">
-        <f t="array" ref="B24">TREND($B$20:$B$21,$A$20:$A$21,B23)</f>
+      <c r="B25" s="2" cm="1">
+        <f t="array" ref="B25">TREND($B$21:$B$22,$A$21:$A$22,B24)</f>
         <v>175132978.72340426</v>
       </c>
-      <c r="C24" s="2" cm="1">
-        <f t="array" ref="C24">TREND($B$20:$B$21,$A$20:$A$21,C23)</f>
+      <c r="C25" s="2" cm="1">
+        <f t="array" ref="C25">TREND($B$21:$B$22,$A$21:$A$22,C24)</f>
         <v>175265957.44680852</v>
       </c>
-      <c r="D24" s="2" cm="1">
-        <f t="array" ref="D24">TREND($B$20:$B$21,$A$20:$A$21,D23)</f>
+      <c r="D25" s="2" cm="1">
+        <f t="array" ref="D25">TREND($B$21:$B$22,$A$21:$A$22,D24)</f>
         <v>175398936.17021278</v>
       </c>
-      <c r="E24" s="2" cm="1">
-        <f t="array" ref="E24">TREND($B$20:$B$21,$A$20:$A$21,E23)</f>
+      <c r="E25" s="2" cm="1">
+        <f t="array" ref="E25">TREND($B$21:$B$22,$A$21:$A$22,E24)</f>
         <v>175531914.893617</v>
       </c>
-      <c r="F24" s="2" cm="1">
-        <f t="array" ref="F24">TREND($B$20:$B$21,$A$20:$A$21,F23)</f>
+      <c r="F25" s="2" cm="1">
+        <f t="array" ref="F25">TREND($B$21:$B$22,$A$21:$A$22,F24)</f>
         <v>175664893.61702126</v>
       </c>
-      <c r="G24" s="2" cm="1">
-        <f t="array" ref="G24">TREND($B$20:$B$21,$A$20:$A$21,G23)</f>
+      <c r="G25" s="2" cm="1">
+        <f t="array" ref="G25">TREND($B$21:$B$22,$A$21:$A$22,G24)</f>
         <v>175797872.34042552</v>
       </c>
-      <c r="H24" s="2" cm="1">
-        <f t="array" ref="H24">TREND($B$20:$B$21,$A$20:$A$21,H23)</f>
+      <c r="H25" s="2" cm="1">
+        <f t="array" ref="H25">TREND($B$21:$B$22,$A$21:$A$22,H24)</f>
         <v>175930851.06382978</v>
       </c>
-      <c r="I24" s="2" cm="1">
-        <f t="array" ref="I24">TREND($B$20:$B$21,$A$20:$A$21,I23)</f>
+      <c r="I25" s="2" cm="1">
+        <f t="array" ref="I25">TREND($B$21:$B$22,$A$21:$A$22,I24)</f>
         <v>176063829.78723404</v>
       </c>
-      <c r="J24" s="2" cm="1">
-        <f t="array" ref="J24">TREND($B$20:$B$21,$A$20:$A$21,J23)</f>
+      <c r="J25" s="2" cm="1">
+        <f t="array" ref="J25">TREND($B$21:$B$22,$A$21:$A$22,J24)</f>
         <v>176196808.5106383</v>
       </c>
-      <c r="K24" s="2" cm="1">
-        <f t="array" ref="K24">TREND($B$20:$B$21,$A$20:$A$21,K23)</f>
+      <c r="K25" s="2" cm="1">
+        <f t="array" ref="K25">TREND($B$21:$B$22,$A$21:$A$22,K24)</f>
         <v>176329787.23404253</v>
       </c>
-      <c r="L24" s="2" cm="1">
-        <f t="array" ref="L24">TREND($B$20:$B$21,$A$20:$A$21,L23)</f>
+      <c r="L25" s="2" cm="1">
+        <f t="array" ref="L25">TREND($B$21:$B$22,$A$21:$A$22,L24)</f>
         <v>176462765.95744681</v>
       </c>
-      <c r="M24" s="2" cm="1">
-        <f t="array" ref="M24">TREND($B$20:$B$21,$A$20:$A$21,M23)</f>
+      <c r="M25" s="2" cm="1">
+        <f t="array" ref="M25">TREND($B$21:$B$22,$A$21:$A$22,M24)</f>
         <v>176595744.68085104</v>
       </c>
-      <c r="N24" s="2" cm="1">
-        <f t="array" ref="N24">TREND($B$20:$B$21,$A$20:$A$21,N23)</f>
+      <c r="N25" s="2" cm="1">
+        <f t="array" ref="N25">TREND($B$21:$B$22,$A$21:$A$22,N24)</f>
         <v>176728723.40425533</v>
       </c>
-      <c r="O24" s="2" cm="1">
-        <f t="array" ref="O24">TREND($B$20:$B$21,$A$20:$A$21,O23)</f>
+      <c r="O25" s="2" cm="1">
+        <f t="array" ref="O25">TREND($B$21:$B$22,$A$21:$A$22,O24)</f>
         <v>176861702.12765956</v>
       </c>
-      <c r="P24" s="2" cm="1">
-        <f t="array" ref="P24">TREND($B$20:$B$21,$A$20:$A$21,P23)</f>
+      <c r="P25" s="2" cm="1">
+        <f t="array" ref="P25">TREND($B$21:$B$22,$A$21:$A$22,P24)</f>
         <v>176994680.85106385</v>
       </c>
-      <c r="Q24" s="2" cm="1">
-        <f t="array" ref="Q24">TREND($B$20:$B$21,$A$20:$A$21,Q23)</f>
+      <c r="Q25" s="2" cm="1">
+        <f t="array" ref="Q25">TREND($B$21:$B$22,$A$21:$A$22,Q24)</f>
         <v>177127659.57446808</v>
       </c>
-      <c r="R24" s="2" cm="1">
-        <f t="array" ref="R24">TREND($B$20:$B$21,$A$20:$A$21,R23)</f>
+      <c r="R25" s="2" cm="1">
+        <f t="array" ref="R25">TREND($B$21:$B$22,$A$21:$A$22,R24)</f>
         <v>177260638.29787236</v>
       </c>
-      <c r="S24" s="2" cm="1">
-        <f t="array" ref="S24">TREND($B$20:$B$21,$A$20:$A$21,S23)</f>
+      <c r="S25" s="2" cm="1">
+        <f t="array" ref="S25">TREND($B$21:$B$22,$A$21:$A$22,S24)</f>
         <v>177393617.02127659</v>
       </c>
-      <c r="T24" s="2" cm="1">
-        <f t="array" ref="T24">TREND($B$20:$B$21,$A$20:$A$21,T23)</f>
+      <c r="T25" s="2" cm="1">
+        <f t="array" ref="T25">TREND($B$21:$B$22,$A$21:$A$22,T24)</f>
         <v>177526595.74468082</v>
       </c>
-      <c r="U24" s="2" cm="1">
-        <f t="array" ref="U24">TREND($B$20:$B$21,$A$20:$A$21,U23)</f>
+      <c r="U25" s="2" cm="1">
+        <f t="array" ref="U25">TREND($B$21:$B$22,$A$21:$A$22,U24)</f>
         <v>177659574.46808511</v>
       </c>
-      <c r="V24" s="2" cm="1">
-        <f t="array" ref="V24">TREND($B$20:$B$21,$A$20:$A$21,V23)</f>
+      <c r="V25" s="2" cm="1">
+        <f t="array" ref="V25">TREND($B$21:$B$22,$A$21:$A$22,V24)</f>
         <v>177792553.19148934</v>
       </c>
-      <c r="W24" s="2" cm="1">
-        <f t="array" ref="W24">TREND($B$20:$B$21,$A$20:$A$21,W23)</f>
+      <c r="W25" s="2" cm="1">
+        <f t="array" ref="W25">TREND($B$21:$B$22,$A$21:$A$22,W24)</f>
         <v>177925531.91489363</v>
       </c>
-      <c r="X24" s="2" cm="1">
-        <f t="array" ref="X24">TREND($B$20:$B$21,$A$20:$A$21,X23)</f>
+      <c r="X25" s="2" cm="1">
+        <f t="array" ref="X25">TREND($B$21:$B$22,$A$21:$A$22,X24)</f>
         <v>178058510.63829786</v>
       </c>
-      <c r="Y24" s="2" cm="1">
-        <f t="array" ref="Y24">TREND($B$20:$B$21,$A$20:$A$21,Y23)</f>
+      <c r="Y25" s="2" cm="1">
+        <f t="array" ref="Y25">TREND($B$21:$B$22,$A$21:$A$22,Y24)</f>
         <v>178191489.36170214</v>
       </c>
-      <c r="Z24" s="2" cm="1">
-        <f t="array" ref="Z24">TREND($B$20:$B$21,$A$20:$A$21,Z23)</f>
+      <c r="Z25" s="2" cm="1">
+        <f t="array" ref="Z25">TREND($B$21:$B$22,$A$21:$A$22,Z24)</f>
         <v>178324468.08510637</v>
       </c>
-      <c r="AA24" s="2" cm="1">
-        <f t="array" ref="AA24">TREND($B$20:$B$21,$A$20:$A$21,AA23)</f>
+      <c r="AA25" s="2" cm="1">
+        <f t="array" ref="AA25">TREND($B$21:$B$22,$A$21:$A$22,AA24)</f>
         <v>178457446.80851066</v>
       </c>
-      <c r="AB24" s="2" cm="1">
-        <f t="array" ref="AB24">TREND($B$20:$B$21,$A$20:$A$21,AB23)</f>
+      <c r="AB25" s="2" cm="1">
+        <f t="array" ref="AB25">TREND($B$21:$B$22,$A$21:$A$22,AB24)</f>
         <v>178590425.53191489</v>
       </c>
-      <c r="AC24" s="2" cm="1">
-        <f t="array" ref="AC24">TREND($B$20:$B$21,$A$20:$A$21,AC23)</f>
+      <c r="AC25" s="2" cm="1">
+        <f t="array" ref="AC25">TREND($B$21:$B$22,$A$21:$A$22,AC24)</f>
         <v>178723404.25531918</v>
       </c>
-      <c r="AD24" s="2" cm="1">
-        <f t="array" ref="AD24">TREND($B$20:$B$21,$A$20:$A$21,AD23)</f>
+      <c r="AD25" s="2" cm="1">
+        <f t="array" ref="AD25">TREND($B$21:$B$22,$A$21:$A$22,AD24)</f>
         <v>178856382.97872341</v>
       </c>
-      <c r="AE24" s="2" cm="1">
-        <f t="array" ref="AE24">TREND($B$20:$B$21,$A$20:$A$21,AE23)</f>
+      <c r="AE25" s="2" cm="1">
+        <f t="array" ref="AE25">TREND($B$21:$B$22,$A$21:$A$22,AE24)</f>
         <v>178989361.70212764</v>
       </c>
-      <c r="AF24" s="2" cm="1">
-        <f t="array" ref="AF24">TREND($B$20:$B$21,$A$20:$A$21,AF23)</f>
+      <c r="AF25" s="2" cm="1">
+        <f t="array" ref="AF25">TREND($B$21:$B$22,$A$21:$A$22,AF24)</f>
         <v>179122340.42553192</v>
       </c>
-      <c r="AG24" s="2" cm="1">
-        <f t="array" ref="AG24">TREND($B$20:$B$21,$A$20:$A$21,AG23)</f>
+      <c r="AG25" s="2" cm="1">
+        <f t="array" ref="AG25">TREND($B$21:$B$22,$A$21:$A$22,AG24)</f>
         <v>179255319.14893615</v>
       </c>
-      <c r="AH24" s="2" cm="1">
-        <f t="array" ref="AH24">TREND($B$20:$B$21,$A$20:$A$21,AH23)</f>
+      <c r="AH25" s="2" cm="1">
+        <f t="array" ref="AH25">TREND($B$21:$B$22,$A$21:$A$22,AH24)</f>
         <v>179388297.87234044</v>
       </c>
-      <c r="AI24" s="2" cm="1">
-        <f t="array" ref="AI24">TREND($B$20:$B$21,$A$20:$A$21,AI23)</f>
+      <c r="AI25" s="2" cm="1">
+        <f t="array" ref="AI25">TREND($B$21:$B$22,$A$21:$A$22,AI24)</f>
         <v>179521276.59574467</v>
       </c>
-      <c r="AJ24" s="2" cm="1">
-        <f t="array" ref="AJ24">TREND($B$20:$B$21,$A$20:$A$21,AJ23)</f>
+      <c r="AJ25" s="2" cm="1">
+        <f t="array" ref="AJ25">TREND($B$21:$B$22,$A$21:$A$22,AJ24)</f>
         <v>179654255.31914896</v>
       </c>
-      <c r="AK24" s="2" cm="1">
-        <f t="array" ref="AK24">TREND($B$20:$B$21,$A$20:$A$21,AK23)</f>
+      <c r="AK25" s="2" cm="1">
+        <f t="array" ref="AK25">TREND($B$21:$B$22,$A$21:$A$22,AK24)</f>
         <v>179787234.04255319</v>
       </c>
-      <c r="AL24" s="2" cm="1">
-        <f t="array" ref="AL24">TREND($B$20:$B$21,$A$20:$A$21,AL23)</f>
+      <c r="AL25" s="2" cm="1">
+        <f t="array" ref="AL25">TREND($B$21:$B$22,$A$21:$A$22,AL24)</f>
         <v>179920212.76595747</v>
       </c>
-      <c r="AM24" s="2" cm="1">
-        <f t="array" ref="AM24">TREND($B$20:$B$21,$A$20:$A$21,AM23)</f>
+      <c r="AM25" s="2" cm="1">
+        <f t="array" ref="AM25">TREND($B$21:$B$22,$A$21:$A$22,AM24)</f>
         <v>180053191.4893617</v>
       </c>
-      <c r="AN24" s="2" cm="1">
-        <f t="array" ref="AN24">TREND($B$20:$B$21,$A$20:$A$21,AN23)</f>
+      <c r="AN25" s="2" cm="1">
+        <f t="array" ref="AN25">TREND($B$21:$B$22,$A$21:$A$22,AN24)</f>
         <v>180186170.21276593</v>
       </c>
-      <c r="AO24" s="2" cm="1">
-        <f t="array" ref="AO24">TREND($B$20:$B$21,$A$20:$A$21,AO23)</f>
+      <c r="AO25" s="2" cm="1">
+        <f t="array" ref="AO25">TREND($B$21:$B$22,$A$21:$A$22,AO24)</f>
         <v>180319148.93617022</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2010</v>
-      </c>
-      <c r="B27">
-        <v>2011</v>
-      </c>
-      <c r="C27">
-        <v>2012</v>
-      </c>
-      <c r="D27">
-        <v>2013</v>
-      </c>
-      <c r="E27">
-        <v>2014</v>
-      </c>
-      <c r="F27">
-        <v>2015</v>
-      </c>
-      <c r="G27">
-        <v>2016</v>
-      </c>
-      <c r="H27">
-        <v>2017</v>
-      </c>
-      <c r="I27">
-        <v>2018</v>
-      </c>
-      <c r="J27">
-        <v>2019</v>
-      </c>
-      <c r="K27">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <f>150*10^6</f>
+        <v>150000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A31">
         <v>2020</v>
       </c>
-      <c r="L27">
+      <c r="B31">
         <v>2021</v>
       </c>
-      <c r="M27">
+      <c r="C31">
         <v>2022</v>
       </c>
-      <c r="N27">
+      <c r="D31">
         <v>2023</v>
       </c>
-      <c r="O27">
+      <c r="E31">
         <v>2024</v>
       </c>
-      <c r="P27">
+      <c r="F31">
         <v>2025</v>
       </c>
-      <c r="Q27">
+      <c r="G31">
         <v>2026</v>
       </c>
-      <c r="R27">
+      <c r="H31">
         <v>2027</v>
       </c>
-      <c r="S27">
+      <c r="I31">
         <v>2028</v>
       </c>
-      <c r="T27">
+      <c r="J31">
         <v>2029</v>
       </c>
-      <c r="U27">
+      <c r="K31">
         <v>2030</v>
       </c>
-      <c r="V27">
+      <c r="L31">
         <v>2031</v>
       </c>
-      <c r="W27">
+      <c r="M31">
         <v>2032</v>
       </c>
-      <c r="X27">
+      <c r="N31">
         <v>2033</v>
       </c>
-      <c r="Y27">
+      <c r="O31">
         <v>2034</v>
       </c>
-      <c r="Z27">
+      <c r="P31">
         <v>2035</v>
       </c>
-      <c r="AA27">
+      <c r="Q31">
         <v>2036</v>
       </c>
-      <c r="AB27">
+      <c r="R31">
         <v>2037</v>
       </c>
-      <c r="AC27">
+      <c r="S31">
         <v>2038</v>
       </c>
-      <c r="AD27">
+      <c r="T31">
         <v>2039</v>
       </c>
-      <c r="AE27">
+      <c r="U31">
         <v>2040</v>
       </c>
-      <c r="AF27">
+      <c r="V31">
         <v>2041</v>
       </c>
-      <c r="AG27">
+      <c r="W31">
         <v>2042</v>
       </c>
-      <c r="AH27">
+      <c r="X31">
         <v>2043</v>
       </c>
-      <c r="AI27">
+      <c r="Y31">
         <v>2044</v>
       </c>
-      <c r="AJ27">
+      <c r="Z31">
         <v>2045</v>
       </c>
-      <c r="AK27">
+      <c r="AA31">
         <v>2046</v>
       </c>
-      <c r="AL27">
+      <c r="AB31">
         <v>2047</v>
       </c>
-      <c r="AM27">
+      <c r="AC31">
         <v>2048</v>
       </c>
-      <c r="AN27">
+      <c r="AD31">
         <v>2049</v>
       </c>
-      <c r="AO27">
+      <c r="AE31">
         <v>2050</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <f>A24/$I$24</f>
-        <v>0.9939577039274925</v>
-      </c>
-      <c r="B28" s="2">
-        <f t="shared" ref="B28:AO28" si="0">B24/$I$24</f>
-        <v>0.99471299093655596</v>
-      </c>
-      <c r="C28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99546827794561943</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99622356495468289</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99697885196374614</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.9977341389728096</v>
-      </c>
-      <c r="G28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99848942598187307</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.99924471299093653</v>
-      </c>
-      <c r="I28" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0007552870090635</v>
-      </c>
-      <c r="K28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0015105740181267</v>
-      </c>
-      <c r="L28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0022658610271904</v>
-      </c>
-      <c r="M28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0030211480362536</v>
-      </c>
-      <c r="N28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0037764350453173</v>
-      </c>
-      <c r="O28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0045317220543806</v>
-      </c>
-      <c r="P28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0052870090634443</v>
-      </c>
-      <c r="Q28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0060422960725075</v>
-      </c>
-      <c r="R28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0067975830815712</v>
-      </c>
-      <c r="S28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0075528700906344</v>
-      </c>
-      <c r="T28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0083081570996977</v>
-      </c>
-      <c r="U28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0090634441087614</v>
-      </c>
-      <c r="V28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0098187311178246</v>
-      </c>
-      <c r="W28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0105740181268883</v>
-      </c>
-      <c r="X28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0113293051359515</v>
-      </c>
-      <c r="Y28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0120845921450152</v>
-      </c>
-      <c r="Z28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0128398791540785</v>
-      </c>
-      <c r="AA28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0135951661631422</v>
-      </c>
-      <c r="AB28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0143504531722054</v>
-      </c>
-      <c r="AC28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0151057401812691</v>
-      </c>
-      <c r="AD28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0158610271903323</v>
-      </c>
-      <c r="AE28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0166163141993956</v>
-      </c>
-      <c r="AF28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0173716012084593</v>
-      </c>
-      <c r="AG28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0181268882175225</v>
-      </c>
-      <c r="AH28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0188821752265862</v>
-      </c>
-      <c r="AI28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0196374622356494</v>
-      </c>
-      <c r="AJ28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0203927492447131</v>
-      </c>
-      <c r="AK28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0211480362537764</v>
-      </c>
-      <c r="AL28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0219033232628401</v>
-      </c>
-      <c r="AM28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0226586102719033</v>
-      </c>
-      <c r="AN28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0234138972809665</v>
-      </c>
-      <c r="AO28" s="2">
-        <f t="shared" si="0"/>
-        <v>1.0241691842900302</v>
-      </c>
-    </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30">
-        <v>700000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="U31" s="2"/>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="9"/>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <f>B29</f>
+        <v>150000000</v>
+      </c>
+      <c r="B32" s="2">
+        <f>$A$32*L25/$K$25</f>
+        <v>150113122.17194575</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" ref="C32:AE32" si="0">$A$32*M25/$K$25</f>
+        <v>150226244.34389141</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>150339366.51583713</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>150452488.68778279</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="0"/>
+        <v>150565610.85972854</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>150678733.03167424</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
+        <v>150791855.20361996</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="0"/>
+        <v>150904977.37556562</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="0"/>
+        <v>151018099.54751131</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="0"/>
+        <v>151131221.71945706</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="0"/>
+        <v>151244343.89140272</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="0"/>
+        <v>151357466.06334844</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="0"/>
+        <v>151470588.23529413</v>
+      </c>
+      <c r="O32" s="2">
+        <f t="shared" si="0"/>
+        <v>151583710.40723985</v>
+      </c>
+      <c r="P32" s="2">
+        <f t="shared" si="0"/>
+        <v>151696832.57918555</v>
+      </c>
+      <c r="Q32" s="2">
+        <f t="shared" si="0"/>
+        <v>151809954.75113127</v>
+      </c>
+      <c r="R32" s="2">
+        <f t="shared" si="0"/>
+        <v>151923076.92307693</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="0"/>
+        <v>152036199.09502268</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="0"/>
+        <v>152149321.26696837</v>
+      </c>
+      <c r="U32" s="2">
+        <f t="shared" si="0"/>
+        <v>152262443.43891403</v>
+      </c>
+      <c r="V32" s="2">
+        <f t="shared" si="0"/>
+        <v>152375565.61085975</v>
+      </c>
+      <c r="W32" s="2">
+        <f t="shared" si="0"/>
+        <v>152488687.78280544</v>
+      </c>
+      <c r="X32" s="2">
+        <f t="shared" si="0"/>
+        <v>152601809.95475119</v>
+      </c>
+      <c r="Y32" s="2">
+        <f t="shared" si="0"/>
+        <v>152714932.12669685</v>
+      </c>
+      <c r="Z32" s="2">
+        <f t="shared" si="0"/>
+        <v>152828054.29864258</v>
+      </c>
+      <c r="AA32" s="2">
+        <f t="shared" si="0"/>
+        <v>152941176.47058824</v>
+      </c>
+      <c r="AB32" s="2">
+        <f t="shared" si="0"/>
+        <v>153054298.64253399</v>
+      </c>
+      <c r="AC32" s="2">
+        <f t="shared" si="0"/>
+        <v>153167420.81447968</v>
+      </c>
+      <c r="AD32" s="2">
+        <f t="shared" si="0"/>
+        <v>153280542.98642534</v>
+      </c>
+      <c r="AE32" s="2">
+        <f t="shared" si="0"/>
+        <v>153393665.15837106</v>
+      </c>
+    </row>
+    <row r="34" spans="11:21" x14ac:dyDescent="0.35">
+      <c r="U34" s="2"/>
+    </row>
+    <row r="36" spans="11:21" x14ac:dyDescent="0.35">
+      <c r="K36" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1539,211 +1437,212 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A8E9EE-75BB-4C67-BE26-F56AE2DF869D}">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B1">
         <f>17*10^6</f>
         <v>17000000</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <f>33*10^9</f>
         <v>33000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>500000000*5</f>
         <v>2500000000</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2">
         <f>B1/B2*B3</f>
         <v>1287878.7878787878</v>
       </c>
-      <c r="D4" s="9">
-        <f>B4/Data!U24</f>
-        <v>7.2491380874614405E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B9">
+        <v>2020</v>
+      </c>
+      <c r="C9">
+        <v>2021</v>
+      </c>
+      <c r="D9">
         <v>2022</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>2023</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>2024</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>2025</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>2026</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>2027</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>2028</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>2029</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>2030</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>2031</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>2032</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>2033</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>2034</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>2035</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>2036</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>2037</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>2038</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>2039</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>2040</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>2041</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>2042</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>2043</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>2044</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>2045</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>2046</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>2047</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>2048</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>2049</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>2050</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="2">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
         <f>$B$4/9</f>
         <v>143097.6430976431</v>
       </c>
-      <c r="C10" s="2">
-        <f>$B$4/9+B10</f>
+      <c r="E10" s="2">
+        <f>$B$4/9+D10</f>
         <v>286195.2861952862</v>
       </c>
-      <c r="D10" s="2">
-        <f t="shared" ref="D10:J10" si="0">$B$4/9+C10</f>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:L10" si="0">$B$4/9+E10</f>
         <v>429292.9292929293</v>
       </c>
-      <c r="E10" s="2">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>572390.5723905724</v>
       </c>
-      <c r="F10" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="0"/>
         <v>715488.21548821544</v>
       </c>
-      <c r="G10" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>858585.85858585848</v>
       </c>
-      <c r="H10" s="2">
+      <c r="J10" s="2">
         <f t="shared" si="0"/>
         <v>1001683.5016835015</v>
       </c>
-      <c r="I10" s="2">
+      <c r="K10" s="2">
         <f t="shared" si="0"/>
         <v>1144781.1447811446</v>
       </c>
-      <c r="J10" s="2">
-        <f t="shared" si="0"/>
-        <v>1287878.7878787876</v>
-      </c>
-      <c r="K10" s="2">
-        <f>$J$10</f>
-        <v>1287878.7878787876</v>
-      </c>
       <c r="L10" s="2">
-        <f t="shared" ref="L10:AD10" si="1">$J$10</f>
+        <f t="shared" si="0"/>
         <v>1287878.7878787876</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="1"/>
+        <f>$L$10</f>
         <v>1287878.7878787876</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N10:AF10" si="1">$L$10</f>
         <v>1287878.7878787876</v>
       </c>
       <c r="O10" s="2">
@@ -1810,130 +1709,17 @@
         <f t="shared" si="1"/>
         <v>1287878.7878787876</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="2">
-        <f>B10/Data!$B$24*Data!$B$30</f>
-        <v>571.95595540318402</v>
-      </c>
-      <c r="C11" s="2">
-        <f>C10/Data!$B$24*Data!$B$30</f>
-        <v>1143.911910806368</v>
-      </c>
-      <c r="D11" s="2">
-        <f>D10/Data!$B$24*Data!$B$30</f>
-        <v>1715.8678662095519</v>
-      </c>
-      <c r="E11" s="2">
-        <f>E10/Data!$B$24*Data!$B$30</f>
-        <v>2287.8238216127361</v>
-      </c>
-      <c r="F11" s="2">
-        <f>F10/Data!$B$24*Data!$B$30</f>
-        <v>2859.7797770159195</v>
-      </c>
-      <c r="G11" s="2">
-        <f>G10/Data!$B$24*Data!$B$30</f>
-        <v>3431.7357324191034</v>
-      </c>
-      <c r="H11" s="2">
-        <f>H10/Data!$B$24*Data!$B$30</f>
-        <v>4003.6916878222869</v>
-      </c>
-      <c r="I11" s="2">
-        <f>I10/Data!$B$24*Data!$B$30</f>
-        <v>4575.6476432254703</v>
-      </c>
-      <c r="J11" s="2">
-        <f>J10/Data!$B$24*Data!$B$30</f>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="K11" s="2">
-        <f>$J$11</f>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="L11" s="2">
-        <f t="shared" ref="L11:AD11" si="2">$J$11</f>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="M11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="N11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="P11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="Q11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="R11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="S11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="T11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="U11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="V11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="W11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="X11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="Y11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="Z11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="AA11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="AB11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="AC11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-      <c r="AD11" s="2">
-        <f t="shared" si="2"/>
-        <v>5147.6035986286543</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K14" s="9"/>
+      <c r="AE10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+      <c r="AF10" s="2">
+        <f t="shared" si="1"/>
+        <v>1287878.7878787876</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="K13" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1945,258 +1731,244 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="34" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="32" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="C1">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="E1">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="F1">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="G1">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="H1">
-        <v>2024</v>
+        <v>2026</v>
       </c>
       <c r="I1">
-        <v>2025</v>
+        <v>2027</v>
       </c>
       <c r="J1">
-        <v>2026</v>
+        <v>2028</v>
       </c>
       <c r="K1">
-        <v>2027</v>
+        <v>2029</v>
       </c>
       <c r="L1">
-        <v>2028</v>
+        <v>2030</v>
       </c>
       <c r="M1">
-        <v>2029</v>
+        <v>2031</v>
       </c>
       <c r="N1">
-        <v>2030</v>
+        <v>2032</v>
       </c>
       <c r="O1">
-        <v>2031</v>
+        <v>2033</v>
       </c>
       <c r="P1">
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="Q1">
-        <v>2033</v>
+        <v>2035</v>
       </c>
       <c r="R1">
-        <v>2034</v>
+        <v>2036</v>
       </c>
       <c r="S1">
-        <v>2035</v>
+        <v>2037</v>
       </c>
       <c r="T1">
-        <v>2036</v>
+        <v>2038</v>
       </c>
       <c r="U1">
-        <v>2037</v>
+        <v>2039</v>
       </c>
       <c r="V1">
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="W1">
-        <v>2039</v>
+        <v>2041</v>
       </c>
       <c r="X1">
-        <v>2040</v>
+        <v>2042</v>
       </c>
       <c r="Y1">
-        <v>2041</v>
+        <v>2043</v>
       </c>
       <c r="Z1">
-        <v>2042</v>
+        <v>2044</v>
       </c>
       <c r="AA1">
-        <v>2043</v>
+        <v>2045</v>
       </c>
       <c r="AB1">
-        <v>2044</v>
+        <v>2046</v>
       </c>
       <c r="AC1">
-        <v>2045</v>
+        <v>2047</v>
       </c>
       <c r="AD1">
-        <v>2046</v>
+        <v>2048</v>
       </c>
       <c r="AE1">
-        <v>2047</v>
+        <v>2049</v>
       </c>
       <c r="AF1">
-        <v>2048</v>
-      </c>
-      <c r="AG1">
-        <v>2049</v>
-      </c>
-      <c r="AH1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3">
-        <f>Data!I28*Data!$B$30</f>
-        <v>700000</v>
+        <f>Data!A32+IIJA!B10</f>
+        <v>150000000</v>
       </c>
       <c r="C2" s="3">
-        <f>Data!J28*Data!$B$30</f>
-        <v>700528.70090634446</v>
+        <f>Data!B32+IIJA!C10</f>
+        <v>150113122.17194575</v>
       </c>
       <c r="D2" s="3">
-        <f>Data!K28*Data!$B$30</f>
-        <v>701057.40181268868</v>
+        <f>Data!C32+IIJA!D10</f>
+        <v>150369341.98698905</v>
       </c>
       <c r="E2" s="3">
-        <f>Data!L28*Data!$B$30</f>
-        <v>701586.10271903325</v>
+        <f>Data!D32+IIJA!E10</f>
+        <v>150625561.80203241</v>
       </c>
       <c r="F2" s="3">
-        <f>Data!M28*Data!$B$30+IIJA!B11</f>
-        <v>702686.75958078075</v>
+        <f>Data!E32+IIJA!F10</f>
+        <v>150881781.61707571</v>
       </c>
       <c r="G2" s="3">
-        <f>Data!N28*Data!$B$30+IIJA!C11</f>
-        <v>703787.41644252848</v>
+        <f>Data!F32+IIJA!G10</f>
+        <v>151138001.43211913</v>
       </c>
       <c r="H2" s="3">
-        <f>Data!O28*Data!$B$30+IIJA!D11</f>
-        <v>704888.07330427598</v>
+        <f>Data!G32+IIJA!H10</f>
+        <v>151394221.24716246</v>
       </c>
       <c r="I2" s="3">
-        <f>Data!P28*Data!$B$30+IIJA!E11</f>
-        <v>705988.73016602371</v>
+        <f>Data!H32+IIJA!I10</f>
+        <v>151650441.06220582</v>
       </c>
       <c r="J2" s="3">
-        <f>Data!Q28*Data!$B$30+IIJA!F11</f>
-        <v>707089.38702777121</v>
+        <f>Data!I32+IIJA!J10</f>
+        <v>151906660.87724912</v>
       </c>
       <c r="K2" s="3">
-        <f>Data!R28*Data!$B$30+IIJA!G11</f>
-        <v>708190.04388951894</v>
+        <f>Data!J32+IIJA!K10</f>
+        <v>152162880.69229245</v>
       </c>
       <c r="L2" s="3">
-        <f>Data!S28*Data!$B$30+IIJA!H11</f>
-        <v>709290.70075126644</v>
+        <f>Data!K32+IIJA!L10</f>
+        <v>152419100.50733584</v>
       </c>
       <c r="M2" s="3">
-        <f>Data!T28*Data!$B$30+IIJA!I11</f>
-        <v>710391.35761301382</v>
+        <f>Data!L32+IIJA!M10</f>
+        <v>152532222.6792815</v>
       </c>
       <c r="N2" s="3">
-        <f>Data!U28*Data!$B$30+IIJA!J11</f>
-        <v>711492.01447476167</v>
+        <f>Data!M32+IIJA!N10</f>
+        <v>152645344.85122722</v>
       </c>
       <c r="O2" s="3">
-        <f>Data!V28*Data!$B$30+IIJA!K11</f>
-        <v>712020.7153811059</v>
+        <f>Data!N32+IIJA!O10</f>
+        <v>152758467.02317291</v>
       </c>
       <c r="P2" s="3">
-        <f>Data!W28*Data!$B$30+IIJA!L11</f>
-        <v>712549.41628745047</v>
+        <f>Data!O32+IIJA!P10</f>
+        <v>152871589.19511864</v>
       </c>
       <c r="Q2" s="3">
-        <f>Data!X28*Data!$B$30+IIJA!M11</f>
-        <v>713078.11719379469</v>
+        <f>Data!P32+IIJA!Q10</f>
+        <v>152984711.36706433</v>
       </c>
       <c r="R2" s="3">
-        <f>Data!Y28*Data!$B$30+IIJA!N11</f>
-        <v>713606.81810013927</v>
+        <f>Data!Q32+IIJA!R10</f>
+        <v>153097833.53901005</v>
       </c>
       <c r="S2" s="3">
-        <f>Data!Z28*Data!$B$30+IIJA!O11</f>
-        <v>714135.51900648361</v>
+        <f>Data!R32+IIJA!S10</f>
+        <v>153210955.71095571</v>
       </c>
       <c r="T2" s="3">
-        <f>Data!AA28*Data!$B$30+IIJA!P11</f>
-        <v>714664.21991282818</v>
+        <f>Data!S32+IIJA!T10</f>
+        <v>153324077.88290146</v>
       </c>
       <c r="U2" s="3">
-        <f>Data!AB28*Data!$B$30+IIJA!Q11</f>
-        <v>715192.9208191724</v>
+        <f>Data!T32+IIJA!U10</f>
+        <v>153437200.05484715</v>
       </c>
       <c r="V2" s="3">
-        <f>Data!AC28*Data!$B$30+IIJA!R11</f>
-        <v>715721.62172551698</v>
+        <f>Data!U32+IIJA!V10</f>
+        <v>153550322.22679281</v>
       </c>
       <c r="W2" s="3">
-        <f>Data!AD28*Data!$B$30+IIJA!S11</f>
-        <v>716250.32263186132</v>
+        <f>Data!V32+IIJA!W10</f>
+        <v>153663444.39873853</v>
       </c>
       <c r="X2" s="3">
-        <f>Data!AE28*Data!$B$30+IIJA!T11</f>
-        <v>716779.02353820554</v>
+        <f>Data!W32+IIJA!X10</f>
+        <v>153776566.57068422</v>
       </c>
       <c r="Y2" s="3">
-        <f>Data!AF28*Data!$B$30+IIJA!U11</f>
-        <v>717307.72444455011</v>
+        <f>Data!X32+IIJA!Y10</f>
+        <v>153889688.74262998</v>
       </c>
       <c r="Z2" s="3">
-        <f>Data!AG28*Data!$B$30+IIJA!V11</f>
-        <v>717836.42535089445</v>
+        <f>Data!Y32+IIJA!Z10</f>
+        <v>154002810.91457564</v>
       </c>
       <c r="AA2" s="3">
-        <f>Data!AH28*Data!$B$30+IIJA!W11</f>
-        <v>718365.12625723903</v>
+        <f>Data!Z32+IIJA!AA10</f>
+        <v>154115933.08652136</v>
       </c>
       <c r="AB2" s="3">
-        <f>Data!AI28*Data!$B$30+IIJA!X11</f>
-        <v>718893.82716358325</v>
+        <f>Data!AA32+IIJA!AB10</f>
+        <v>154229055.25846702</v>
       </c>
       <c r="AC2" s="3">
-        <f>Data!AJ28*Data!$B$30+IIJA!Y11</f>
-        <v>719422.52806992782</v>
+        <f>Data!AB32+IIJA!AC10</f>
+        <v>154342177.43041277</v>
       </c>
       <c r="AD2" s="3">
-        <f>Data!AK28*Data!$B$30+IIJA!Z11</f>
-        <v>719951.22897627216</v>
+        <f>Data!AC32+IIJA!AD10</f>
+        <v>154455299.60235846</v>
       </c>
       <c r="AE2" s="3">
-        <f>Data!AL28*Data!$B$30+IIJA!AA11</f>
-        <v>720479.92988261674</v>
+        <f>Data!AD32+IIJA!AE10</f>
+        <v>154568421.77430412</v>
       </c>
       <c r="AF2" s="3">
-        <f>Data!AM28*Data!$B$30+IIJA!AB11</f>
-        <v>721008.63078896096</v>
-      </c>
-      <c r="AG2" s="3">
-        <f>Data!AN28*Data!$B$30+IIJA!AC11</f>
-        <v>721537.33169530518</v>
-      </c>
-      <c r="AH2" s="3">
-        <f>Data!AO28*Data!$B$30+IIJA!AD11</f>
-        <v>722066.03260164987</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="N4" s="3"/>
+        <f>Data!AE32+IIJA!AF10</f>
+        <v>154681543.94624984</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="L4" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>